<commit_message>
finished growth, cleaned data
</commit_message>
<xml_diff>
--- a/data/growth_data.xlsx
+++ b/data/growth_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="381">
   <si>
     <t>common_name</t>
   </si>
@@ -316,9 +316,6 @@
     <t>Edsall-1999-TransAmFishSoc</t>
   </si>
   <si>
-    <t>0.0533</t>
-  </si>
-  <si>
     <t>Common wolffish</t>
   </si>
   <si>
@@ -334,9 +331,6 @@
     <t>McCarthy-etal-1998-AquacultureInt</t>
   </si>
   <si>
-    <t>The small size is larvae</t>
-  </si>
-  <si>
     <t>0.113</t>
   </si>
   <si>
@@ -971,12 +965,6 @@
   </si>
   <si>
     <t>11.209</t>
-  </si>
-  <si>
-    <t>0.270</t>
-  </si>
-  <si>
-    <t>0.1196</t>
   </si>
   <si>
     <t>63.1</t>
@@ -1548,11 +1536,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V61"/>
+  <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,22 +1571,22 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -1660,10 +1648,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
@@ -1672,28 +1660,28 @@
         <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="O2" s="3">
         <v>2</v>
       </c>
       <c r="P2" s="3">
-        <v>11744000</v>
+        <v>11744</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>43</v>
@@ -1713,7 +1701,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B3" s="3">
         <v>14</v>
@@ -1722,10 +1710,10 @@
         <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>24</v>
@@ -1734,22 +1722,22 @@
         <v>21</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>32</v>
@@ -1770,7 +1758,7 @@
         <v>43</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>22</v>
@@ -1778,19 +1766,19 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B4" s="3">
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>296</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>24</v>
@@ -1799,22 +1787,22 @@
         <v>21</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>32</v>
@@ -1835,7 +1823,7 @@
         <v>43</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="V4" s="3" t="s">
         <v>22</v>
@@ -1843,19 +1831,19 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B5" s="3">
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>24</v>
@@ -1864,22 +1852,22 @@
         <v>21</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>32</v>
@@ -1900,7 +1888,7 @@
         <v>43</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>22</v>
@@ -1908,19 +1896,19 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B6" s="3">
         <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>28</v>
@@ -1929,22 +1917,22 @@
         <v>27</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>212</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>36</v>
@@ -1962,13 +1950,13 @@
         <v>43</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1988,25 +1976,25 @@
         <v>39</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>217</v>
-      </c>
       <c r="O7" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P7" s="3">
         <v>9500</v>
@@ -2024,7 +2012,7 @@
         <v>6</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="V7" s="3" t="s">
         <v>30</v>
@@ -2047,25 +2035,25 @@
         <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J8" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>217</v>
-      </c>
       <c r="O8" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P8" s="3">
         <v>9500</v>
@@ -2083,7 +2071,7 @@
         <v>6</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="V8" s="3" t="s">
         <v>30</v>
@@ -2106,25 +2094,25 @@
         <v>39</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J9" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>217</v>
-      </c>
       <c r="O9" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P9" s="3">
         <v>9500</v>
@@ -2142,7 +2130,7 @@
         <v>6</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="V9" s="3" t="s">
         <v>30</v>
@@ -2165,25 +2153,25 @@
         <v>39</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>217</v>
-      </c>
       <c r="O10" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P10" s="3">
         <v>9500</v>
@@ -2201,7 +2189,7 @@
         <v>6</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="V10" s="3" t="s">
         <v>30</v>
@@ -2215,40 +2203,40 @@
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="H11" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="O11" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="P11" s="3">
         <v>100000</v>
@@ -2263,7 +2251,7 @@
         <v>43</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="V11" s="3" t="s">
         <v>42</v>
@@ -2271,16 +2259,16 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B12" s="3">
         <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E12" s="3">
         <v>17</v>
@@ -2292,25 +2280,25 @@
         <v>45</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P12" s="3">
         <v>9100</v>
@@ -2325,10 +2313,10 @@
         <v>43</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="V12" s="3" t="s">
         <v>47</v>
@@ -2336,19 +2324,19 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B13" s="3">
         <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>44</v>
@@ -2357,25 +2345,25 @@
         <v>45</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P13" s="3">
         <v>9100</v>
@@ -2390,10 +2378,10 @@
         <v>43</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="V13" s="3" t="s">
         <v>47</v>
@@ -2401,19 +2389,19 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B14" s="3">
         <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>44</v>
@@ -2422,25 +2410,25 @@
         <v>45</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P14" s="3">
         <v>9100</v>
@@ -2455,10 +2443,10 @@
         <v>43</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="V14" s="3" t="s">
         <v>47</v>
@@ -2466,7 +2454,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B15" s="3">
         <v>25</v>
@@ -2475,7 +2463,7 @@
         <v>179</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E15" s="3">
         <v>251</v>
@@ -2487,25 +2475,25 @@
         <v>45</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P15" s="3">
         <v>9100</v>
@@ -2520,10 +2508,10 @@
         <v>43</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="V15" s="3" t="s">
         <v>47</v>
@@ -2534,7 +2522,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -2548,22 +2536,22 @@
         <v>52</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J16" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="L16" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="N16" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O16" s="4" t="s">
         <v>36</v>
@@ -2581,10 +2569,10 @@
         <v>10</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V16" s="4" t="s">
         <v>48</v>
@@ -2609,22 +2597,22 @@
         <v>52</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J17" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="M17" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="L17" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="N17" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>36</v>
@@ -2642,10 +2630,10 @@
         <v>10</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="U17" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V17" s="4" t="s">
         <v>48</v>
@@ -2659,10 +2647,10 @@
         <v>26</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E18" s="3">
         <v>49</v>
@@ -2674,25 +2662,25 @@
         <v>56</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P18" s="3">
         <v>96800</v>
@@ -2715,16 +2703,16 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E19" s="3">
         <v>143</v>
@@ -2736,25 +2724,25 @@
         <v>60</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J19" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>238</v>
-      </c>
       <c r="M19" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P19" s="3">
         <v>10000</v>
@@ -2772,7 +2760,7 @@
         <v>43</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="V19" s="3" t="s">
         <v>58</v>
@@ -2789,10 +2777,10 @@
         <v>65</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>63</v>
@@ -2801,22 +2789,22 @@
         <v>64</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J20" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>241</v>
-      </c>
       <c r="N20" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="O20" s="3">
         <v>2</v>
@@ -2831,7 +2819,7 @@
         <v>33</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="T20" s="3" t="s">
         <v>43</v>
@@ -2859,25 +2847,25 @@
         <v>68</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J21" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="M21" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="L21" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="N21" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P21" s="4">
         <v>46800</v>
@@ -2889,7 +2877,7 @@
         <v>9</v>
       </c>
       <c r="S21" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="T21" s="4" t="s">
         <v>18</v>
@@ -2918,25 +2906,25 @@
         <v>68</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J22" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="M22" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="N22" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P22" s="4">
         <v>46800</v>
@@ -2948,7 +2936,7 @@
         <v>9</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="T22" s="4" t="s">
         <v>18</v>
@@ -2966,13 +2954,13 @@
         <v>72</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
@@ -2982,25 +2970,25 @@
         <v>76</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J23" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="O23" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="O23" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="P23" s="4">
         <v>60000</v>
@@ -3012,10 +3000,10 @@
         <v>28</v>
       </c>
       <c r="S23" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="U23" s="4"/>
       <c r="V23" s="4" t="s">
@@ -3030,7 +3018,7 @@
         <v>77</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -3042,25 +3030,25 @@
         <v>80</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J24" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="M24" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="N24" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="O24" s="4" t="s">
         <v>250</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="O24" s="4" t="s">
-        <v>252</v>
       </c>
       <c r="P24" s="4">
         <v>3900</v>
@@ -3084,7 +3072,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B25" s="4">
         <v>31</v>
@@ -3093,10 +3081,10 @@
         <v>84</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
@@ -3106,25 +3094,25 @@
         <v>82</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P25" s="4">
         <v>45000</v>
@@ -3142,7 +3130,7 @@
         <v>43</v>
       </c>
       <c r="U25" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="V25" s="4" t="s">
         <v>85</v>
@@ -3159,7 +3147,7 @@
         <v>89</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E26" s="4">
         <v>46</v>
@@ -3172,25 +3160,25 @@
         <v>87</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="P26" s="4">
         <v>1900</v>
@@ -3225,10 +3213,10 @@
         <v>97</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4" t="s">
@@ -3238,25 +3226,25 @@
         <v>95</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P27" s="4">
         <v>19000</v>
@@ -3280,47 +3268,47 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="H28" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="I28" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L28" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="N28" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="M28" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>209</v>
-      </c>
       <c r="O28" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="P28" s="4">
         <v>23600</v>
@@ -3337,186 +3325,180 @@
       <c r="T28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U28" s="4" t="s">
+      <c r="U28" s="4"/>
+      <c r="V28" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P29" s="3">
+        <v>652</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="V29" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="V28" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="4">
-        <v>11</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="P29" s="4">
-        <v>23600</v>
-      </c>
-      <c r="Q29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U29" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="V29" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>109</v>
+        <v>135</v>
+      </c>
+      <c r="B30" s="3">
+        <v>17</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>107</v>
+        <v>322</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>324</v>
+        <v>125</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>323</v>
+        <v>143</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I30" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I30" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="J30" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="O30" s="3" t="s">
-        <v>32</v>
+      <c r="J30" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="P30" s="3">
-        <v>652</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="U30" s="3" t="s">
-        <v>325</v>
+        <v>96000</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>2</v>
+      </c>
+      <c r="R30" s="5">
+        <v>16</v>
+      </c>
+      <c r="S30" s="5">
+        <v>9</v>
+      </c>
+      <c r="T30" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="V30" s="3" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B31" s="3">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P31" s="3">
         <v>96000</v>
@@ -3534,51 +3516,51 @@
         <v>89</v>
       </c>
       <c r="V31" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>132</v>
+        <v>34</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>146</v>
+        <v>325</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P32" s="3">
         <v>96000</v>
@@ -3596,51 +3578,51 @@
         <v>89</v>
       </c>
       <c r="V32" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>328</v>
+        <v>131</v>
+      </c>
+      <c r="C33" s="3">
+        <v>17</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>329</v>
+        <v>145</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P33" s="3">
         <v>96000</v>
@@ -3658,51 +3640,51 @@
         <v>89</v>
       </c>
       <c r="V33" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="3">
-        <v>17</v>
+        <v>132</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>326</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="I34" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P34" s="3">
         <v>96000</v>
@@ -3720,51 +3702,51 @@
         <v>89</v>
       </c>
       <c r="V34" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
+      </c>
+      <c r="C35" s="3">
+        <v>309</v>
+      </c>
+      <c r="D35" s="3">
+        <v>447</v>
+      </c>
+      <c r="E35" s="3">
+        <v>648</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P35" s="3">
         <v>96000</v>
@@ -3782,51 +3764,51 @@
         <v>89</v>
       </c>
       <c r="V35" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="C36" s="3">
-        <v>309</v>
+        <v>628</v>
       </c>
       <c r="D36" s="3">
-        <v>447</v>
+        <v>874</v>
       </c>
       <c r="E36" s="3">
-        <v>648</v>
+        <v>1217</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P36" s="3">
         <v>96000</v>
@@ -3844,51 +3826,51 @@
         <v>89</v>
       </c>
       <c r="V36" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="C37" s="3">
-        <v>628</v>
+        <v>1503</v>
       </c>
       <c r="D37" s="3">
-        <v>874</v>
+        <v>2213</v>
       </c>
       <c r="E37" s="3">
-        <v>1217</v>
+        <v>3154</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P37" s="3">
         <v>96000</v>
@@ -3906,113 +3888,116 @@
         <v>89</v>
       </c>
       <c r="V37" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>136</v>
+        <v>110</v>
+      </c>
+      <c r="B38" s="3">
+        <v>14</v>
       </c>
       <c r="C38" s="3">
-        <v>1503</v>
-      </c>
-      <c r="D38" s="3">
-        <v>2213</v>
-      </c>
-      <c r="E38" s="3">
-        <v>3154</v>
+        <v>8</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="F38" s="3">
+        <v>35</v>
       </c>
       <c r="G38" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="O38" s="3">
+        <v>4</v>
+      </c>
+      <c r="P38" s="3">
+        <v>320000</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="V38" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="N38" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="O38" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="P38" s="3">
-        <v>96000</v>
-      </c>
-      <c r="Q38" s="5">
-        <v>2</v>
-      </c>
-      <c r="R38" s="5">
-        <v>16</v>
-      </c>
-      <c r="S38" s="5">
-        <v>9</v>
-      </c>
-      <c r="T38" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="V38" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="3">
-        <v>14</v>
+        <v>149</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C39" s="3">
-        <v>8</v>
+        <v>136</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
+      </c>
+      <c r="E39" s="3">
+        <v>451</v>
       </c>
       <c r="F39" s="3">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J39" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L39" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="K39" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="L39" s="3" t="s">
+      <c r="M39" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N39" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="M39" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="N39" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="O39" s="3">
         <v>4</v>
@@ -4030,10 +4015,10 @@
         <v>43</v>
       </c>
       <c r="T39" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V39" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -4044,40 +4029,40 @@
         <v>150</v>
       </c>
       <c r="C40" s="3">
-        <v>136</v>
+        <v>3000</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E40" s="3">
-        <v>451</v>
+        <v>4600</v>
       </c>
       <c r="F40" s="3">
-        <v>300</v>
+        <v>4000</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J40" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L40" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="K40" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="L40" s="3" t="s">
+      <c r="M40" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N40" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="M40" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="N40" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="O40" s="3">
         <v>4</v>
@@ -4095,10 +4080,10 @@
         <v>43</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V40" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -4106,108 +4091,111 @@
         <v>153</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="3">
-        <v>3000</v>
+        <v>158</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E41" s="3">
-        <v>4600</v>
-      </c>
-      <c r="F41" s="3">
-        <v>4000</v>
+        <v>347</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="G41" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P41" s="3">
+        <v>25000</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U41" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="V41" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="M41" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="N41" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="O41" s="3">
-        <v>4</v>
-      </c>
-      <c r="P41" s="3">
-        <v>320000</v>
-      </c>
-      <c r="Q41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T41" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="V41" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="E42" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M42" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="M42" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="N42" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O42" s="3" t="s">
         <v>36</v>
@@ -4228,54 +4216,54 @@
         <v>37</v>
       </c>
       <c r="U42" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="V42" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>337</v>
-      </c>
       <c r="F43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H43" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="I43" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O43" s="3" t="s">
         <v>36</v>
@@ -4296,54 +4284,54 @@
         <v>37</v>
       </c>
       <c r="U43" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="V43" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>36</v>
+        <v>165</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O44" s="3" t="s">
         <v>36</v>
@@ -4364,54 +4352,54 @@
         <v>37</v>
       </c>
       <c r="U44" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="V44" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>167</v>
+        <v>339</v>
+      </c>
+      <c r="F45" s="3">
+        <v>54</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O45" s="3" t="s">
         <v>36</v>
@@ -4432,54 +4420,54 @@
         <v>37</v>
       </c>
       <c r="U45" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="V45" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>347</v>
-      </c>
       <c r="E46" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F46" s="3">
-        <v>54</v>
+        <v>499</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O46" s="3" t="s">
         <v>36</v>
@@ -4500,60 +4488,57 @@
         <v>37</v>
       </c>
       <c r="U46" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="V46" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>165</v>
+        <v>350</v>
+      </c>
+      <c r="B47" s="3">
+        <v>16</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>344</v>
+        <v>168</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="F47" s="3">
-        <v>499</v>
+        <v>348</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>168</v>
+        <v>259</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>199</v>
+        <v>260</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="N47" s="5" t="s">
-        <v>209</v>
+        <v>262</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>263</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>36</v>
+        <v>244</v>
       </c>
       <c r="P47" s="3">
-        <v>25000</v>
+        <v>5263</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>43</v>
@@ -4565,75 +4550,69 @@
         <v>43</v>
       </c>
       <c r="T47" s="3" t="s">
-        <v>37</v>
+        <v>241</v>
       </c>
       <c r="U47" s="3" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="V47" s="3" t="s">
-        <v>123</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="B48" s="3">
-        <v>16</v>
-      </c>
-      <c r="C48" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="H48" s="3" t="s">
-        <v>261</v>
+        <v>124</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="K48" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N48" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="L48" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="M48" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="N48" s="3" t="s">
+      <c r="O48" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="O48" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="P48" s="3">
-        <v>5263</v>
-      </c>
-      <c r="Q48" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R48" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S48" s="3" t="s">
-        <v>43</v>
+        <v>582</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>-2</v>
+      </c>
+      <c r="R48" s="3">
+        <v>8</v>
+      </c>
+      <c r="S48" s="3">
+        <v>3</v>
       </c>
       <c r="T48" s="3" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
       <c r="V48" s="3" t="s">
         <v>169</v>
@@ -4641,40 +4620,40 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>173</v>
+        <v>352</v>
+      </c>
+      <c r="B49" s="3">
+        <v>9</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N49" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P49" s="3">
         <v>582</v>
@@ -4689,107 +4668,107 @@
         <v>3</v>
       </c>
       <c r="T49" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="U49" s="3" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="V49" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>356</v>
+        <v>173</v>
       </c>
       <c r="B50" s="3">
-        <v>9</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>358</v>
+        <v>33</v>
+      </c>
+      <c r="F50" s="3">
+        <v>10</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>266</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>250</v>
+        <v>209</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>227</v>
+        <v>268</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="O50" s="3" t="s">
-        <v>267</v>
+        <v>218</v>
+      </c>
+      <c r="O50" s="3">
+        <v>4</v>
       </c>
       <c r="P50" s="3">
-        <v>582</v>
+        <v>68000</v>
       </c>
       <c r="Q50" s="3">
-        <v>-2</v>
+        <v>17</v>
       </c>
       <c r="R50" s="3">
-        <v>8</v>
-      </c>
-      <c r="S50" s="3">
-        <v>3</v>
-      </c>
-      <c r="T50" s="3" t="s">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="T50" s="3">
+        <v>14</v>
       </c>
       <c r="U50" s="3" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="V50" s="3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B51" s="3">
         <v>33</v>
       </c>
       <c r="F51" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I51" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M51" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="J51" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="M51" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="N51" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O51" s="3">
         <v>4</v>
@@ -4804,51 +4783,51 @@
         <v>32</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="T51" s="3">
         <v>14</v>
       </c>
       <c r="U51" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="V51" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B52" s="3">
         <v>33</v>
       </c>
       <c r="F52" s="3">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I52" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M52" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="J52" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="M52" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="N52" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O52" s="3">
         <v>4</v>
@@ -4863,51 +4842,51 @@
         <v>32</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="T52" s="3">
         <v>14</v>
       </c>
       <c r="U52" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="V52" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B53" s="3">
         <v>33</v>
       </c>
       <c r="F53" s="3">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I53" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M53" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="J53" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L53" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="M53" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="N53" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O53" s="3">
         <v>4</v>
@@ -4922,110 +4901,107 @@
         <v>32</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="T53" s="3">
         <v>14</v>
       </c>
       <c r="U53" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="V53" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>178</v>
+        <v>367</v>
       </c>
       <c r="B54" s="3">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F54" s="3">
-        <v>200</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="J54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="O54" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P54" s="6">
+        <v>4800</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>10</v>
+      </c>
+      <c r="R54" s="6">
+        <v>22</v>
+      </c>
+      <c r="S54" s="6">
+        <v>16</v>
+      </c>
+      <c r="T54" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="V54" s="4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>6</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="K54" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="M54" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="N54" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="O54" s="3">
-        <v>4</v>
-      </c>
-      <c r="P54" s="3">
-        <v>68000</v>
-      </c>
-      <c r="Q54" s="3">
-        <v>17</v>
-      </c>
-      <c r="R54" s="3">
-        <v>32</v>
-      </c>
-      <c r="S54" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="T54" s="3">
-        <v>14</v>
-      </c>
-      <c r="U54" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="V54" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="B55" s="3">
-        <v>28</v>
-      </c>
       <c r="F55" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M55" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O55" s="6" t="s">
         <v>36</v>
@@ -5046,42 +5022,42 @@
         <v>43</v>
       </c>
       <c r="V55" s="4" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>6</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>271</v>
+        <v>4</v>
+      </c>
+      <c r="B56" s="3">
+        <v>23</v>
       </c>
       <c r="F56" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M56" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O56" s="6" t="s">
         <v>36</v>
@@ -5102,42 +5078,42 @@
         <v>43</v>
       </c>
       <c r="V56" s="4" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B57" s="3">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F57" s="3">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M57" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O57" s="6" t="s">
         <v>36</v>
@@ -5158,101 +5134,101 @@
         <v>43</v>
       </c>
       <c r="V57" s="4" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
-        <v>3</v>
+      <c r="A58" s="3" t="s">
+        <v>376</v>
       </c>
       <c r="B58" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F58" s="3">
-        <v>100</v>
-      </c>
-      <c r="G58" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="I58" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="H58" s="6" t="s">
+      <c r="J58" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="L58" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="M58" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="N58" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="O58" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="P58" s="8">
+        <v>300</v>
+      </c>
+      <c r="Q58" s="8">
+        <v>16</v>
+      </c>
+      <c r="R58" s="8">
+        <v>25</v>
+      </c>
+      <c r="S58" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="I58" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="J58" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="K58" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="L58" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="M58" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="N58" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="O58" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P58" s="6">
-        <v>4800</v>
-      </c>
-      <c r="Q58" s="6">
-        <v>10</v>
-      </c>
-      <c r="R58" s="6">
-        <v>22</v>
-      </c>
-      <c r="S58" s="6">
-        <v>16</v>
-      </c>
       <c r="T58" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V58" s="4" t="s">
-        <v>370</v>
+      <c r="V58" s="8" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B59" s="3">
         <v>27</v>
       </c>
       <c r="F59" s="3">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="J59" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M59" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N59" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O59" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="P59" s="8">
         <v>300</v>
@@ -5264,51 +5240,51 @@
         <v>25</v>
       </c>
       <c r="S59" s="8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="T59" s="5" t="s">
         <v>43</v>
       </c>
       <c r="V59" s="8" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B60" s="3">
         <v>27</v>
       </c>
       <c r="F60" s="3">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="J60" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M60" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N60" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O60" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="P60" s="8">
         <v>300</v>
@@ -5320,69 +5296,13 @@
         <v>25</v>
       </c>
       <c r="S60" s="8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="T60" s="5" t="s">
         <v>43</v>
       </c>
       <c r="V60" s="8" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="B61" s="3">
-        <v>27</v>
-      </c>
-      <c r="F61" s="3">
-        <v>36</v>
-      </c>
-      <c r="G61" s="8" t="s">
         <v>375</v>
-      </c>
-      <c r="H61" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="I61" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="J61" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="K61" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="L61" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="M61" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="N61" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="O61" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="P61" s="8">
-        <v>300</v>
-      </c>
-      <c r="Q61" s="8">
-        <v>16</v>
-      </c>
-      <c r="R61" s="8">
-        <v>25</v>
-      </c>
-      <c r="S61" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="T61" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="V61" s="8" t="s">
-        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first update of scalig draft v2. New analysis coming...
</commit_message>
<xml_diff>
--- a/data/growth_data.xlsx
+++ b/data/growth_data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48063D80-4BAB-E04B-8642-C340A0019301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="13455" windowHeight="6915"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="33880" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3968" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3986" uniqueCount="607">
   <si>
     <t>common_name</t>
   </si>
@@ -1813,9 +1814,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>SGR growth from Fig 1; Sizes from Table 1; Temperature not from Fishbase but from this paper: Effects of water temperature on feeding and growth of juvenile marbled flounder Pseudopleuronectes yokohamae under laboratory conditions: evaluation by group- and individual-based methods</t>
-  </si>
-  <si>
     <t>Demersal</t>
   </si>
   <si>
@@ -1835,16 +1833,22 @@
   </si>
   <si>
     <t>Reef-associated; oceanodromous</t>
+  </si>
+  <si>
+    <t>13.5</t>
+  </si>
+  <si>
+    <t>SGR growth from Fig 1; Sizes from Table 1; Environmental temperature from Joh, M., Nakaya, M., Yoshida, N. &amp; Takatsu, T. (2013). Interannual growth differences and growth-selective survival in larvae and juveniles of marbled sole Pseudopleuronectes yokohamae. Marine Ecology Progress Series, 494, 267–279. AND Mitamura, H., Arai, N., Hori, M., Uchida, K., Kajiyama, M. &amp; Ishii, M. (2020). Occurrence of a temperate coastal flatfish, the marbled flounder Pseudopleuronectes yokohamae, at high water temperatures in a shallow bay in summer detected by acoustic telemetry. Fish Sci, 86, 77–85.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1862,6 +1866,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2012,6 +2022,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2047,6 +2074,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2222,44 +2266,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O214" sqref="O214"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="35.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="35.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="3"/>
+    <col min="11" max="11" width="14.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" style="3" customWidth="1"/>
     <col min="22" max="22" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="117.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.140625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="37.42578125" style="3" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="3"/>
+    <col min="23" max="23" width="117.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.1640625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="37.5" style="3" customWidth="1"/>
+    <col min="26" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>121</v>
       </c>
@@ -2336,7 +2380,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>214</v>
       </c>
@@ -2374,7 +2418,7 @@
         <v>80</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>81</v>
@@ -2397,11 +2441,11 @@
       <c r="U2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="3">
-        <v>11</v>
+      <c r="V2" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X2" s="3">
         <v>1</v>
@@ -2410,7 +2454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>216</v>
       </c>
@@ -2448,7 +2492,7 @@
         <v>80</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>81</v>
@@ -2471,11 +2515,11 @@
       <c r="U3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V3" s="3">
-        <v>11</v>
+      <c r="V3" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X3" s="3">
         <v>1</v>
@@ -2484,7 +2528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>218</v>
       </c>
@@ -2522,7 +2566,7 @@
         <v>80</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>81</v>
@@ -2545,11 +2589,11 @@
       <c r="U4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V4" s="3">
-        <v>11</v>
+      <c r="V4" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X4" s="3">
         <v>1</v>
@@ -2558,7 +2602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>220</v>
       </c>
@@ -2596,7 +2640,7 @@
         <v>80</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>81</v>
@@ -2619,11 +2663,11 @@
       <c r="U5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V5" s="3">
-        <v>11</v>
+      <c r="V5" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X5" s="3">
         <v>1</v>
@@ -2632,7 +2676,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>222</v>
       </c>
@@ -2670,7 +2714,7 @@
         <v>80</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>81</v>
@@ -2693,11 +2737,11 @@
       <c r="U6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V6" s="3">
-        <v>11</v>
+      <c r="V6" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X6" s="3">
         <v>1</v>
@@ -2706,7 +2750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>224</v>
       </c>
@@ -2744,7 +2788,7 @@
         <v>80</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>81</v>
@@ -2767,11 +2811,11 @@
       <c r="U7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V7" s="3">
-        <v>11</v>
+      <c r="V7" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X7" s="3">
         <v>1</v>
@@ -2780,7 +2824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>226</v>
       </c>
@@ -2818,7 +2862,7 @@
         <v>80</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>81</v>
@@ -2841,11 +2885,11 @@
       <c r="U8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V8" s="3">
-        <v>11</v>
+      <c r="V8" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X8" s="3">
         <v>1</v>
@@ -2854,7 +2898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>228</v>
       </c>
@@ -2892,7 +2936,7 @@
         <v>80</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>81</v>
@@ -2915,11 +2959,11 @@
       <c r="U9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V9" s="3">
-        <v>11</v>
+      <c r="V9" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X9" s="3">
         <v>1</v>
@@ -2928,7 +2972,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>230</v>
       </c>
@@ -2966,7 +3010,7 @@
         <v>80</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>81</v>
@@ -2989,11 +3033,11 @@
       <c r="U10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V10" s="3">
-        <v>11</v>
+      <c r="V10" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X10" s="3">
         <v>1</v>
@@ -3002,7 +3046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>232</v>
       </c>
@@ -3040,7 +3084,7 @@
         <v>80</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>81</v>
@@ -3063,11 +3107,11 @@
       <c r="U11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V11" s="3">
-        <v>11</v>
+      <c r="V11" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X11" s="3">
         <v>1</v>
@@ -3076,7 +3120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>234</v>
       </c>
@@ -3114,7 +3158,7 @@
         <v>80</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>81</v>
@@ -3137,11 +3181,11 @@
       <c r="U12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V12" s="3">
-        <v>11</v>
+      <c r="V12" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X12" s="3">
         <v>1</v>
@@ -3150,7 +3194,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>236</v>
       </c>
@@ -3188,7 +3232,7 @@
         <v>80</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>81</v>
@@ -3211,11 +3255,11 @@
       <c r="U13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V13" s="3">
-        <v>11</v>
+      <c r="V13" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X13" s="3">
         <v>1</v>
@@ -3224,7 +3268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>238</v>
       </c>
@@ -3262,7 +3306,7 @@
         <v>80</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>81</v>
@@ -3285,11 +3329,11 @@
       <c r="U14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V14" s="3">
-        <v>11</v>
+      <c r="V14" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X14" s="3">
         <v>1</v>
@@ -3298,7 +3342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>240</v>
       </c>
@@ -3336,7 +3380,7 @@
         <v>80</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>81</v>
@@ -3359,11 +3403,11 @@
       <c r="U15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V15" s="3">
-        <v>11</v>
+      <c r="V15" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X15" s="3">
         <v>1</v>
@@ -3372,7 +3416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>242</v>
       </c>
@@ -3410,7 +3454,7 @@
         <v>80</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>81</v>
@@ -3433,11 +3477,11 @@
       <c r="U16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V16" s="3">
-        <v>11</v>
+      <c r="V16" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X16" s="3">
         <v>1</v>
@@ -3446,7 +3490,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>244</v>
       </c>
@@ -3484,7 +3528,7 @@
         <v>80</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>81</v>
@@ -3507,11 +3551,11 @@
       <c r="U17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V17" s="3">
-        <v>11</v>
+      <c r="V17" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X17" s="3">
         <v>1</v>
@@ -3520,7 +3564,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>246</v>
       </c>
@@ -3558,7 +3602,7 @@
         <v>80</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>81</v>
@@ -3581,11 +3625,11 @@
       <c r="U18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V18" s="3">
-        <v>11</v>
+      <c r="V18" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X18" s="3">
         <v>1</v>
@@ -3594,7 +3638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>6</v>
       </c>
@@ -3632,7 +3676,7 @@
         <v>80</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>81</v>
@@ -3655,11 +3699,11 @@
       <c r="U19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V19" s="3">
-        <v>11</v>
+      <c r="V19" s="3" t="s">
+        <v>605</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="X19" s="3">
         <v>1</v>
@@ -3668,7 +3712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>208</v>
       </c>
@@ -3700,7 +3744,7 @@
         <v>80</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>85</v>
@@ -3736,7 +3780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>250</v>
       </c>
@@ -3768,7 +3812,7 @@
         <v>80</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O21" s="3" t="s">
         <v>85</v>
@@ -3804,7 +3848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>252</v>
       </c>
@@ -3836,7 +3880,7 @@
         <v>80</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O22" s="3" t="s">
         <v>85</v>
@@ -3872,7 +3916,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>254</v>
       </c>
@@ -3904,7 +3948,7 @@
         <v>80</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>85</v>
@@ -3940,7 +3984,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>256</v>
       </c>
@@ -3972,7 +4016,7 @@
         <v>80</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>85</v>
@@ -4008,7 +4052,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>258</v>
       </c>
@@ -4040,7 +4084,7 @@
         <v>80</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>85</v>
@@ -4076,7 +4120,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>260</v>
       </c>
@@ -4108,7 +4152,7 @@
         <v>80</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>85</v>
@@ -4144,7 +4188,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>262</v>
       </c>
@@ -4176,7 +4220,7 @@
         <v>80</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O27" s="3" t="s">
         <v>85</v>
@@ -4212,7 +4256,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>264</v>
       </c>
@@ -4244,7 +4288,7 @@
         <v>80</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>85</v>
@@ -4280,7 +4324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>266</v>
       </c>
@@ -4312,7 +4356,7 @@
         <v>80</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O29" s="3" t="s">
         <v>85</v>
@@ -4348,7 +4392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>268</v>
       </c>
@@ -4380,7 +4424,7 @@
         <v>80</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>85</v>
@@ -4416,7 +4460,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>270</v>
       </c>
@@ -4448,7 +4492,7 @@
         <v>80</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>85</v>
@@ -4484,7 +4528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>272</v>
       </c>
@@ -4516,7 +4560,7 @@
         <v>80</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O32" s="3" t="s">
         <v>85</v>
@@ -4552,7 +4596,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>274</v>
       </c>
@@ -4584,7 +4628,7 @@
         <v>80</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O33" s="3" t="s">
         <v>85</v>
@@ -4620,7 +4664,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>276</v>
       </c>
@@ -4652,7 +4696,7 @@
         <v>80</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O34" s="3" t="s">
         <v>85</v>
@@ -4688,7 +4732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>278</v>
       </c>
@@ -4720,7 +4764,7 @@
         <v>80</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O35" s="3" t="s">
         <v>85</v>
@@ -4756,7 +4800,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>280</v>
       </c>
@@ -4788,7 +4832,7 @@
         <v>80</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O36" s="3" t="s">
         <v>85</v>
@@ -4824,7 +4868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>282</v>
       </c>
@@ -4856,7 +4900,7 @@
         <v>80</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O37" s="3" t="s">
         <v>85</v>
@@ -4892,7 +4936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>284</v>
       </c>
@@ -4924,7 +4968,7 @@
         <v>80</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O38" s="3" t="s">
         <v>85</v>
@@ -4960,7 +5004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>286</v>
       </c>
@@ -4992,7 +5036,7 @@
         <v>80</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O39" s="3" t="s">
         <v>85</v>
@@ -5028,7 +5072,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>288</v>
       </c>
@@ -5066,7 +5110,7 @@
         <v>80</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O40" s="3" t="s">
         <v>86</v>
@@ -5102,7 +5146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>290</v>
       </c>
@@ -5140,7 +5184,7 @@
         <v>80</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O41" s="3" t="s">
         <v>86</v>
@@ -5176,7 +5220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>292</v>
       </c>
@@ -5214,7 +5258,7 @@
         <v>80</v>
       </c>
       <c r="N42" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O42" s="3" t="s">
         <v>86</v>
@@ -5250,7 +5294,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>294</v>
       </c>
@@ -5288,7 +5332,7 @@
         <v>80</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O43" s="3" t="s">
         <v>86</v>
@@ -5324,7 +5368,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>296</v>
       </c>
@@ -5362,7 +5406,7 @@
         <v>80</v>
       </c>
       <c r="N44" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O44" s="3" t="s">
         <v>86</v>
@@ -5398,7 +5442,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>298</v>
       </c>
@@ -5436,7 +5480,7 @@
         <v>80</v>
       </c>
       <c r="N45" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O45" s="3" t="s">
         <v>86</v>
@@ -5472,7 +5516,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>300</v>
       </c>
@@ -5510,7 +5554,7 @@
         <v>80</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O46" s="3" t="s">
         <v>86</v>
@@ -5546,7 +5590,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>302</v>
       </c>
@@ -5584,7 +5628,7 @@
         <v>80</v>
       </c>
       <c r="N47" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O47" s="3" t="s">
         <v>86</v>
@@ -5620,7 +5664,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>304</v>
       </c>
@@ -5658,7 +5702,7 @@
         <v>80</v>
       </c>
       <c r="N48" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O48" s="3" t="s">
         <v>86</v>
@@ -5694,7 +5738,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>306</v>
       </c>
@@ -5732,7 +5776,7 @@
         <v>80</v>
       </c>
       <c r="N49" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O49" s="3" t="s">
         <v>86</v>
@@ -5768,7 +5812,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>308</v>
       </c>
@@ -5806,7 +5850,7 @@
         <v>80</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O50" s="3" t="s">
         <v>86</v>
@@ -5842,7 +5886,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>310</v>
       </c>
@@ -5880,7 +5924,7 @@
         <v>80</v>
       </c>
       <c r="N51" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O51" s="3" t="s">
         <v>86</v>
@@ -5916,7 +5960,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>312</v>
       </c>
@@ -5954,7 +5998,7 @@
         <v>80</v>
       </c>
       <c r="N52" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O52" s="3" t="s">
         <v>86</v>
@@ -5990,7 +6034,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>314</v>
       </c>
@@ -6028,7 +6072,7 @@
         <v>80</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O53" s="3" t="s">
         <v>86</v>
@@ -6064,7 +6108,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>316</v>
       </c>
@@ -6102,7 +6146,7 @@
         <v>80</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O54" s="3" t="s">
         <v>86</v>
@@ -6138,7 +6182,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>318</v>
       </c>
@@ -6176,7 +6220,7 @@
         <v>80</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O55" s="3" t="s">
         <v>86</v>
@@ -6212,7 +6256,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>320</v>
       </c>
@@ -6250,7 +6294,7 @@
         <v>80</v>
       </c>
       <c r="N56" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O56" s="3" t="s">
         <v>86</v>
@@ -6286,7 +6330,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>322</v>
       </c>
@@ -6324,7 +6368,7 @@
         <v>80</v>
       </c>
       <c r="N57" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O57" s="3" t="s">
         <v>86</v>
@@ -6360,7 +6404,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>324</v>
       </c>
@@ -6398,7 +6442,7 @@
         <v>80</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O58" s="3" t="s">
         <v>86</v>
@@ -6434,7 +6478,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>326</v>
       </c>
@@ -6472,7 +6516,7 @@
         <v>80</v>
       </c>
       <c r="N59" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O59" s="3" t="s">
         <v>86</v>
@@ -6508,7 +6552,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>328</v>
       </c>
@@ -6542,7 +6586,7 @@
         <v>94</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O60" s="4" t="s">
         <v>81</v>
@@ -6578,7 +6622,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>330</v>
       </c>
@@ -6612,7 +6656,7 @@
         <v>94</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O61" s="4" t="s">
         <v>81</v>
@@ -6648,7 +6692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>332</v>
       </c>
@@ -6680,7 +6724,7 @@
         <v>94</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O62" s="4" t="s">
         <v>81</v>
@@ -6716,7 +6760,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>334</v>
       </c>
@@ -6748,7 +6792,7 @@
         <v>94</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O63" s="4" t="s">
         <v>81</v>
@@ -6784,7 +6828,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>336</v>
       </c>
@@ -6816,7 +6860,7 @@
         <v>94</v>
       </c>
       <c r="N64" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O64" s="4" t="s">
         <v>81</v>
@@ -6852,7 +6896,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>338</v>
       </c>
@@ -6884,7 +6928,7 @@
         <v>94</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O65" s="4" t="s">
         <v>81</v>
@@ -6920,7 +6964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>340</v>
       </c>
@@ -6954,7 +6998,7 @@
         <v>94</v>
       </c>
       <c r="N66" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O66" s="4" t="s">
         <v>81</v>
@@ -6990,7 +7034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>342</v>
       </c>
@@ -7024,7 +7068,7 @@
         <v>94</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O67" s="4" t="s">
         <v>81</v>
@@ -7060,7 +7104,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>344</v>
       </c>
@@ -7092,7 +7136,7 @@
         <v>94</v>
       </c>
       <c r="N68" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O68" s="4" t="s">
         <v>81</v>
@@ -7128,7 +7172,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>346</v>
       </c>
@@ -7160,7 +7204,7 @@
         <v>94</v>
       </c>
       <c r="N69" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O69" s="4" t="s">
         <v>81</v>
@@ -7196,7 +7240,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>348</v>
       </c>
@@ -7228,7 +7272,7 @@
         <v>94</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O70" s="4" t="s">
         <v>81</v>
@@ -7264,7 +7308,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>350</v>
       </c>
@@ -7296,7 +7340,7 @@
         <v>94</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O71" s="4" t="s">
         <v>81</v>
@@ -7332,7 +7376,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>352</v>
       </c>
@@ -7364,7 +7408,7 @@
         <v>94</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O72" s="4" t="s">
         <v>81</v>
@@ -7400,7 +7444,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>354</v>
       </c>
@@ -7432,7 +7476,7 @@
         <v>94</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O73" s="4" t="s">
         <v>81</v>
@@ -7468,7 +7512,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>51</v>
       </c>
@@ -7507,7 +7551,7 @@
         <v>94</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O74" s="3" t="s">
         <v>77</v>
@@ -7543,7 +7587,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>168</v>
       </c>
@@ -7582,7 +7626,7 @@
         <v>94</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O75" s="3" t="s">
         <v>77</v>
@@ -7618,7 +7662,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>138</v>
       </c>
@@ -7657,7 +7701,7 @@
         <v>94</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O76" s="3" t="s">
         <v>77</v>
@@ -7693,7 +7737,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>138</v>
       </c>
@@ -7732,7 +7776,7 @@
         <v>94</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O77" s="3" t="s">
         <v>77</v>
@@ -7768,7 +7812,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>169</v>
       </c>
@@ -7806,7 +7850,7 @@
         <v>94</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O78" s="3" t="s">
         <v>77</v>
@@ -7842,7 +7886,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>170</v>
       </c>
@@ -7880,7 +7924,7 @@
         <v>94</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O79" s="3" t="s">
         <v>77</v>
@@ -7916,7 +7960,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>171</v>
       </c>
@@ -7954,7 +7998,7 @@
         <v>94</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O80" s="3" t="s">
         <v>77</v>
@@ -7990,7 +8034,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>172</v>
       </c>
@@ -8028,7 +8072,7 @@
         <v>94</v>
       </c>
       <c r="N81" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O81" s="3" t="s">
         <v>77</v>
@@ -8064,7 +8108,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>173</v>
       </c>
@@ -8102,7 +8146,7 @@
         <v>94</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O82" s="3" t="s">
         <v>77</v>
@@ -8138,7 +8182,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>136</v>
       </c>
@@ -8176,7 +8220,7 @@
         <v>94</v>
       </c>
       <c r="N83" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O83" s="3" t="s">
         <v>77</v>
@@ -8212,7 +8256,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>174</v>
       </c>
@@ -8250,7 +8294,7 @@
         <v>94</v>
       </c>
       <c r="N84" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O84" s="3" t="s">
         <v>77</v>
@@ -8286,7 +8330,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>175</v>
       </c>
@@ -8324,7 +8368,7 @@
         <v>94</v>
       </c>
       <c r="N85" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O85" s="3" t="s">
         <v>77</v>
@@ -8360,7 +8404,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>359</v>
       </c>
@@ -8392,7 +8436,7 @@
         <v>96</v>
       </c>
       <c r="N86" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O86" s="5" t="s">
         <v>81</v>
@@ -8428,7 +8472,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>361</v>
       </c>
@@ -8460,7 +8504,7 @@
         <v>96</v>
       </c>
       <c r="N87" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O87" s="5" t="s">
         <v>81</v>
@@ -8496,7 +8540,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>363</v>
       </c>
@@ -8528,7 +8572,7 @@
         <v>96</v>
       </c>
       <c r="N88" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O88" s="5" t="s">
         <v>81</v>
@@ -8564,7 +8608,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>365</v>
       </c>
@@ -8596,7 +8640,7 @@
         <v>96</v>
       </c>
       <c r="N89" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O89" s="5" t="s">
         <v>81</v>
@@ -8632,7 +8676,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>367</v>
       </c>
@@ -8665,7 +8709,7 @@
         <v>96</v>
       </c>
       <c r="N90" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O90" s="5" t="s">
         <v>81</v>
@@ -8701,7 +8745,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>369</v>
       </c>
@@ -8734,7 +8778,7 @@
         <v>96</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O91" s="5" t="s">
         <v>81</v>
@@ -8770,7 +8814,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>371</v>
       </c>
@@ -8802,7 +8846,7 @@
         <v>96</v>
       </c>
       <c r="N92" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O92" s="5" t="s">
         <v>81</v>
@@ -8838,7 +8882,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>373</v>
       </c>
@@ -8870,7 +8914,7 @@
         <v>96</v>
       </c>
       <c r="N93" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O93" s="5" t="s">
         <v>81</v>
@@ -8906,7 +8950,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>375</v>
       </c>
@@ -8938,7 +8982,7 @@
         <v>96</v>
       </c>
       <c r="N94" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O94" s="5" t="s">
         <v>81</v>
@@ -8974,7 +9018,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>377</v>
       </c>
@@ -9006,7 +9050,7 @@
         <v>96</v>
       </c>
       <c r="N95" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O95" s="5" t="s">
         <v>81</v>
@@ -9042,7 +9086,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>379</v>
       </c>
@@ -9074,7 +9118,7 @@
         <v>96</v>
       </c>
       <c r="N96" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O96" s="5" t="s">
         <v>81</v>
@@ -9110,7 +9154,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>381</v>
       </c>
@@ -9142,7 +9186,7 @@
         <v>96</v>
       </c>
       <c r="N97" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O97" s="5" t="s">
         <v>81</v>
@@ -9178,7 +9222,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>383</v>
       </c>
@@ -9210,7 +9254,7 @@
         <v>96</v>
       </c>
       <c r="N98" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O98" s="5" t="s">
         <v>81</v>
@@ -9246,7 +9290,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>385</v>
       </c>
@@ -9278,7 +9322,7 @@
         <v>96</v>
       </c>
       <c r="N99" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O99" s="5" t="s">
         <v>81</v>
@@ -9314,7 +9358,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>387</v>
       </c>
@@ -9346,7 +9390,7 @@
         <v>96</v>
       </c>
       <c r="N100" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O100" s="5" t="s">
         <v>81</v>
@@ -9382,7 +9426,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>389</v>
       </c>
@@ -9414,7 +9458,7 @@
         <v>96</v>
       </c>
       <c r="N101" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O101" s="5" t="s">
         <v>81</v>
@@ -9450,7 +9494,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>391</v>
       </c>
@@ -9482,7 +9526,7 @@
         <v>96</v>
       </c>
       <c r="N102" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O102" s="5" t="s">
         <v>81</v>
@@ -9518,7 +9562,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>393</v>
       </c>
@@ -9550,7 +9594,7 @@
         <v>96</v>
       </c>
       <c r="N103" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O103" s="5" t="s">
         <v>81</v>
@@ -9586,7 +9630,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>395</v>
       </c>
@@ -9618,7 +9662,7 @@
         <v>96</v>
       </c>
       <c r="N104" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O104" s="5" t="s">
         <v>81</v>
@@ -9654,7 +9698,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>397</v>
       </c>
@@ -9686,7 +9730,7 @@
         <v>96</v>
       </c>
       <c r="N105" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O105" s="5" t="s">
         <v>81</v>
@@ -9722,7 +9766,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>399</v>
       </c>
@@ -9754,7 +9798,7 @@
         <v>96</v>
       </c>
       <c r="N106" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O106" s="5" t="s">
         <v>81</v>
@@ -9790,7 +9834,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>401</v>
       </c>
@@ -9822,7 +9866,7 @@
         <v>96</v>
       </c>
       <c r="N107" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O107" s="5" t="s">
         <v>81</v>
@@ -9858,7 +9902,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>403</v>
       </c>
@@ -9890,7 +9934,7 @@
         <v>96</v>
       </c>
       <c r="N108" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O108" s="5" t="s">
         <v>81</v>
@@ -9926,7 +9970,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>405</v>
       </c>
@@ -9958,7 +10002,7 @@
         <v>96</v>
       </c>
       <c r="N109" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O109" s="5" t="s">
         <v>81</v>
@@ -9994,7 +10038,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>407</v>
       </c>
@@ -10026,7 +10070,7 @@
         <v>96</v>
       </c>
       <c r="N110" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O110" s="5" t="s">
         <v>81</v>
@@ -10062,7 +10106,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>409</v>
       </c>
@@ -10094,7 +10138,7 @@
         <v>96</v>
       </c>
       <c r="N111" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O111" s="5" t="s">
         <v>81</v>
@@ -10130,7 +10174,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>411</v>
       </c>
@@ -10162,7 +10206,7 @@
         <v>96</v>
       </c>
       <c r="N112" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O112" s="5" t="s">
         <v>81</v>
@@ -10198,7 +10242,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>413</v>
       </c>
@@ -10230,7 +10274,7 @@
         <v>96</v>
       </c>
       <c r="N113" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O113" s="5" t="s">
         <v>81</v>
@@ -10266,7 +10310,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>415</v>
       </c>
@@ -10298,7 +10342,7 @@
         <v>96</v>
       </c>
       <c r="N114" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O114" s="5" t="s">
         <v>81</v>
@@ -10334,7 +10378,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>417</v>
       </c>
@@ -10366,7 +10410,7 @@
         <v>96</v>
       </c>
       <c r="N115" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O115" s="5" t="s">
         <v>81</v>
@@ -10402,7 +10446,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>419</v>
       </c>
@@ -10434,7 +10478,7 @@
         <v>96</v>
       </c>
       <c r="N116" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O116" s="5" t="s">
         <v>81</v>
@@ -10470,7 +10514,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>421</v>
       </c>
@@ -10502,7 +10546,7 @@
         <v>96</v>
       </c>
       <c r="N117" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O117" s="5" t="s">
         <v>81</v>
@@ -10538,7 +10582,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>423</v>
       </c>
@@ -10570,7 +10614,7 @@
         <v>96</v>
       </c>
       <c r="N118" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O118" s="5" t="s">
         <v>81</v>
@@ -10606,7 +10650,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>425</v>
       </c>
@@ -10638,7 +10682,7 @@
         <v>96</v>
       </c>
       <c r="N119" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O119" s="5" t="s">
         <v>81</v>
@@ -10674,7 +10718,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>427</v>
       </c>
@@ -10706,7 +10750,7 @@
         <v>80</v>
       </c>
       <c r="N120" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O120" s="5" t="s">
         <v>81</v>
@@ -10742,7 +10786,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>429</v>
       </c>
@@ -10774,7 +10818,7 @@
         <v>80</v>
       </c>
       <c r="N121" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O121" s="5" t="s">
         <v>81</v>
@@ -10810,7 +10854,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>431</v>
       </c>
@@ -10842,7 +10886,7 @@
         <v>80</v>
       </c>
       <c r="N122" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O122" s="5" t="s">
         <v>81</v>
@@ -10878,7 +10922,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>433</v>
       </c>
@@ -10910,7 +10954,7 @@
         <v>80</v>
       </c>
       <c r="N123" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O123" s="5" t="s">
         <v>81</v>
@@ -10946,7 +10990,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>435</v>
       </c>
@@ -10978,7 +11022,7 @@
         <v>80</v>
       </c>
       <c r="N124" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O124" s="5" t="s">
         <v>81</v>
@@ -11014,7 +11058,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>437</v>
       </c>
@@ -11046,7 +11090,7 @@
         <v>80</v>
       </c>
       <c r="N125" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O125" s="5" t="s">
         <v>81</v>
@@ -11082,7 +11126,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>439</v>
       </c>
@@ -11114,7 +11158,7 @@
         <v>80</v>
       </c>
       <c r="N126" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O126" s="5" t="s">
         <v>81</v>
@@ -11150,7 +11194,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>441</v>
       </c>
@@ -11182,7 +11226,7 @@
         <v>80</v>
       </c>
       <c r="N127" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O127" s="5" t="s">
         <v>81</v>
@@ -11218,7 +11262,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>443</v>
       </c>
@@ -11250,7 +11294,7 @@
         <v>80</v>
       </c>
       <c r="N128" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O128" s="5" t="s">
         <v>81</v>
@@ -11286,7 +11330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>445</v>
       </c>
@@ -11318,7 +11362,7 @@
         <v>80</v>
       </c>
       <c r="N129" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O129" s="5" t="s">
         <v>81</v>
@@ -11354,7 +11398,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>447</v>
       </c>
@@ -11386,7 +11430,7 @@
         <v>80</v>
       </c>
       <c r="N130" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O130" s="5" t="s">
         <v>81</v>
@@ -11422,7 +11466,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>449</v>
       </c>
@@ -11454,7 +11498,7 @@
         <v>80</v>
       </c>
       <c r="N131" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O131" s="5" t="s">
         <v>81</v>
@@ -11490,7 +11534,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>451</v>
       </c>
@@ -11522,7 +11566,7 @@
         <v>80</v>
       </c>
       <c r="N132" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O132" s="5" t="s">
         <v>81</v>
@@ -11558,7 +11602,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>453</v>
       </c>
@@ -11590,7 +11634,7 @@
         <v>80</v>
       </c>
       <c r="N133" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O133" s="5" t="s">
         <v>81</v>
@@ -11626,7 +11670,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>455</v>
       </c>
@@ -11658,7 +11702,7 @@
         <v>80</v>
       </c>
       <c r="N134" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O134" s="5" t="s">
         <v>81</v>
@@ -11694,7 +11738,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>457</v>
       </c>
@@ -11726,7 +11770,7 @@
         <v>80</v>
       </c>
       <c r="N135" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O135" s="5" t="s">
         <v>81</v>
@@ -11762,7 +11806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>459</v>
       </c>
@@ -11794,7 +11838,7 @@
         <v>80</v>
       </c>
       <c r="N136" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O136" s="5" t="s">
         <v>81</v>
@@ -11830,7 +11874,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>461</v>
       </c>
@@ -11862,7 +11906,7 @@
         <v>96</v>
       </c>
       <c r="N137" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O137" s="5" t="s">
         <v>81</v>
@@ -11898,7 +11942,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>463</v>
       </c>
@@ -11930,7 +11974,7 @@
         <v>96</v>
       </c>
       <c r="N138" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O138" s="5" t="s">
         <v>81</v>
@@ -11966,7 +12010,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>465</v>
       </c>
@@ -11998,7 +12042,7 @@
         <v>96</v>
       </c>
       <c r="N139" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O139" s="5" t="s">
         <v>81</v>
@@ -12034,7 +12078,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>467</v>
       </c>
@@ -12066,7 +12110,7 @@
         <v>96</v>
       </c>
       <c r="N140" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O140" s="5" t="s">
         <v>81</v>
@@ -12102,7 +12146,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>469</v>
       </c>
@@ -12134,7 +12178,7 @@
         <v>96</v>
       </c>
       <c r="N141" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O141" s="5" t="s">
         <v>81</v>
@@ -12170,7 +12214,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>471</v>
       </c>
@@ -12202,7 +12246,7 @@
         <v>96</v>
       </c>
       <c r="N142" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O142" s="5" t="s">
         <v>81</v>
@@ -12238,7 +12282,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>473</v>
       </c>
@@ -12270,7 +12314,7 @@
         <v>96</v>
       </c>
       <c r="N143" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O143" s="5" t="s">
         <v>81</v>
@@ -12306,7 +12350,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>475</v>
       </c>
@@ -12338,7 +12382,7 @@
         <v>96</v>
       </c>
       <c r="N144" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O144" s="5" t="s">
         <v>81</v>
@@ -12374,7 +12418,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>477</v>
       </c>
@@ -12406,7 +12450,7 @@
         <v>96</v>
       </c>
       <c r="N145" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O145" s="5" t="s">
         <v>81</v>
@@ -12442,7 +12486,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>479</v>
       </c>
@@ -12474,7 +12518,7 @@
         <v>96</v>
       </c>
       <c r="N146" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O146" s="5" t="s">
         <v>81</v>
@@ -12510,7 +12554,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>481</v>
       </c>
@@ -12542,7 +12586,7 @@
         <v>96</v>
       </c>
       <c r="N147" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O147" s="5" t="s">
         <v>81</v>
@@ -12578,7 +12622,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>483</v>
       </c>
@@ -12610,7 +12654,7 @@
         <v>96</v>
       </c>
       <c r="N148" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O148" s="5" t="s">
         <v>81</v>
@@ -12646,7 +12690,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>485</v>
       </c>
@@ -12678,7 +12722,7 @@
         <v>96</v>
       </c>
       <c r="N149" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O149" s="5" t="s">
         <v>81</v>
@@ -12714,7 +12758,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>487</v>
       </c>
@@ -12746,7 +12790,7 @@
         <v>96</v>
       </c>
       <c r="N150" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O150" s="5" t="s">
         <v>81</v>
@@ -12782,7 +12826,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>489</v>
       </c>
@@ -12814,7 +12858,7 @@
         <v>96</v>
       </c>
       <c r="N151" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O151" s="5" t="s">
         <v>81</v>
@@ -12850,7 +12894,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>477</v>
       </c>
@@ -12882,7 +12926,7 @@
         <v>96</v>
       </c>
       <c r="N152" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O152" s="5" t="s">
         <v>81</v>
@@ -12918,7 +12962,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>492</v>
       </c>
@@ -12950,7 +12994,7 @@
         <v>96</v>
       </c>
       <c r="N153" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O153" s="5" t="s">
         <v>81</v>
@@ -12986,7 +13030,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>494</v>
       </c>
@@ -13018,7 +13062,7 @@
         <v>96</v>
       </c>
       <c r="N154" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O154" s="5" t="s">
         <v>81</v>
@@ -13054,7 +13098,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>496</v>
       </c>
@@ -13086,7 +13130,7 @@
         <v>96</v>
       </c>
       <c r="N155" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O155" s="5" t="s">
         <v>81</v>
@@ -13122,7 +13166,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>498</v>
       </c>
@@ -13154,7 +13198,7 @@
         <v>96</v>
       </c>
       <c r="N156" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O156" s="5" t="s">
         <v>81</v>
@@ -13190,7 +13234,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>500</v>
       </c>
@@ -13222,7 +13266,7 @@
         <v>96</v>
       </c>
       <c r="N157" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O157" s="5" t="s">
         <v>81</v>
@@ -13258,7 +13302,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>502</v>
       </c>
@@ -13290,7 +13334,7 @@
         <v>96</v>
       </c>
       <c r="N158" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O158" s="5" t="s">
         <v>81</v>
@@ -13326,7 +13370,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>504</v>
       </c>
@@ -13358,7 +13402,7 @@
         <v>96</v>
       </c>
       <c r="N159" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O159" s="5" t="s">
         <v>81</v>
@@ -13394,7 +13438,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>506</v>
       </c>
@@ -13426,7 +13470,7 @@
         <v>96</v>
       </c>
       <c r="N160" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O160" s="5" t="s">
         <v>81</v>
@@ -13462,7 +13506,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>508</v>
       </c>
@@ -13494,7 +13538,7 @@
         <v>96</v>
       </c>
       <c r="N161" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O161" s="5" t="s">
         <v>81</v>
@@ -13530,7 +13574,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>510</v>
       </c>
@@ -13562,7 +13606,7 @@
         <v>96</v>
       </c>
       <c r="N162" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O162" s="5" t="s">
         <v>81</v>
@@ -13598,7 +13642,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>512</v>
       </c>
@@ -13630,7 +13674,7 @@
         <v>96</v>
       </c>
       <c r="N163" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O163" s="5" t="s">
         <v>81</v>
@@ -13666,7 +13710,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>514</v>
       </c>
@@ -13698,7 +13742,7 @@
         <v>96</v>
       </c>
       <c r="N164" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O164" s="5" t="s">
         <v>81</v>
@@ -13734,7 +13778,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>516</v>
       </c>
@@ -13766,7 +13810,7 @@
         <v>96</v>
       </c>
       <c r="N165" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O165" s="5" t="s">
         <v>81</v>
@@ -13802,7 +13846,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>518</v>
       </c>
@@ -13834,7 +13878,7 @@
         <v>96</v>
       </c>
       <c r="N166" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O166" s="5" t="s">
         <v>81</v>
@@ -13870,7 +13914,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>520</v>
       </c>
@@ -13902,7 +13946,7 @@
         <v>96</v>
       </c>
       <c r="N167" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O167" s="5" t="s">
         <v>81</v>
@@ -13938,7 +13982,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>522</v>
       </c>
@@ -13970,7 +14014,7 @@
         <v>96</v>
       </c>
       <c r="N168" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O168" s="5" t="s">
         <v>81</v>
@@ -14006,7 +14050,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>524</v>
       </c>
@@ -14038,7 +14082,7 @@
         <v>96</v>
       </c>
       <c r="N169" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O169" s="5" t="s">
         <v>81</v>
@@ -14074,7 +14118,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>526</v>
       </c>
@@ -14106,7 +14150,7 @@
         <v>96</v>
       </c>
       <c r="N170" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O170" s="5" t="s">
         <v>81</v>
@@ -14142,7 +14186,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>528</v>
       </c>
@@ -14174,7 +14218,7 @@
         <v>96</v>
       </c>
       <c r="N171" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O171" s="5" t="s">
         <v>81</v>
@@ -14210,7 +14254,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>530</v>
       </c>
@@ -14242,7 +14286,7 @@
         <v>96</v>
       </c>
       <c r="N172" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O172" s="3" t="s">
         <v>85</v>
@@ -14278,7 +14322,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>531</v>
       </c>
@@ -14310,7 +14354,7 @@
         <v>96</v>
       </c>
       <c r="N173" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O173" s="3" t="s">
         <v>85</v>
@@ -14346,7 +14390,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>532</v>
       </c>
@@ -14378,7 +14422,7 @@
         <v>96</v>
       </c>
       <c r="N174" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O174" s="3" t="s">
         <v>85</v>
@@ -14414,7 +14458,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>533</v>
       </c>
@@ -14446,7 +14490,7 @@
         <v>96</v>
       </c>
       <c r="N175" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O175" s="3" t="s">
         <v>85</v>
@@ -14482,7 +14526,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>534</v>
       </c>
@@ -14514,7 +14558,7 @@
         <v>96</v>
       </c>
       <c r="N176" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O176" s="3" t="s">
         <v>85</v>
@@ -14550,7 +14594,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>535</v>
       </c>
@@ -14582,7 +14626,7 @@
         <v>96</v>
       </c>
       <c r="N177" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O177" s="3" t="s">
         <v>85</v>
@@ -14618,7 +14662,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
         <v>536</v>
       </c>
@@ -14650,7 +14694,7 @@
         <v>96</v>
       </c>
       <c r="N178" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O178" s="3" t="s">
         <v>85</v>
@@ -14686,7 +14730,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>537</v>
       </c>
@@ -14718,7 +14762,7 @@
         <v>96</v>
       </c>
       <c r="N179" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O179" s="3" t="s">
         <v>85</v>
@@ -14754,7 +14798,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
         <v>538</v>
       </c>
@@ -14786,7 +14830,7 @@
         <v>96</v>
       </c>
       <c r="N180" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O180" s="3" t="s">
         <v>85</v>
@@ -14822,7 +14866,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>539</v>
       </c>
@@ -14854,7 +14898,7 @@
         <v>96</v>
       </c>
       <c r="N181" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O181" s="3" t="s">
         <v>85</v>
@@ -14890,7 +14934,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>187</v>
       </c>
@@ -14922,7 +14966,7 @@
         <v>96</v>
       </c>
       <c r="N182" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O182" s="3" t="s">
         <v>86</v>
@@ -14958,7 +15002,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>60</v>
       </c>
@@ -14990,7 +15034,7 @@
         <v>96</v>
       </c>
       <c r="N183" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O183" s="3" t="s">
         <v>86</v>
@@ -15026,7 +15070,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
         <v>188</v>
       </c>
@@ -15058,7 +15102,7 @@
         <v>96</v>
       </c>
       <c r="N184" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O184" s="3" t="s">
         <v>86</v>
@@ -15094,7 +15138,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>189</v>
       </c>
@@ -15126,7 +15170,7 @@
         <v>96</v>
       </c>
       <c r="N185" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O185" s="3" t="s">
         <v>86</v>
@@ -15162,7 +15206,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
         <v>190</v>
       </c>
@@ -15194,7 +15238,7 @@
         <v>96</v>
       </c>
       <c r="N186" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O186" s="3" t="s">
         <v>86</v>
@@ -15230,7 +15274,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>191</v>
       </c>
@@ -15262,7 +15306,7 @@
         <v>96</v>
       </c>
       <c r="N187" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O187" s="3" t="s">
         <v>86</v>
@@ -15298,7 +15342,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
         <v>61</v>
       </c>
@@ -15330,7 +15374,7 @@
         <v>96</v>
       </c>
       <c r="N188" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O188" s="3" t="s">
         <v>86</v>
@@ -15366,7 +15410,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
         <v>192</v>
       </c>
@@ -15398,7 +15442,7 @@
         <v>96</v>
       </c>
       <c r="N189" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O189" s="3" t="s">
         <v>86</v>
@@ -15434,7 +15478,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
         <v>193</v>
       </c>
@@ -15466,7 +15510,7 @@
         <v>96</v>
       </c>
       <c r="N190" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O190" s="3" t="s">
         <v>86</v>
@@ -15502,7 +15546,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
         <v>194</v>
       </c>
@@ -15534,7 +15578,7 @@
         <v>96</v>
       </c>
       <c r="N191" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O191" s="3" t="s">
         <v>86</v>
@@ -15570,7 +15614,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
         <v>195</v>
       </c>
@@ -15602,7 +15646,7 @@
         <v>96</v>
       </c>
       <c r="N192" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O192" s="3" t="s">
         <v>86</v>
@@ -15638,7 +15682,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>62</v>
       </c>
@@ -15670,7 +15714,7 @@
         <v>96</v>
       </c>
       <c r="N193" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O193" s="3" t="s">
         <v>86</v>
@@ -15706,7 +15750,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>196</v>
       </c>
@@ -15738,7 +15782,7 @@
         <v>96</v>
       </c>
       <c r="N194" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O194" s="3" t="s">
         <v>86</v>
@@ -15774,7 +15818,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>197</v>
       </c>
@@ -15806,7 +15850,7 @@
         <v>96</v>
       </c>
       <c r="N195" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O195" s="3" t="s">
         <v>86</v>
@@ -15842,7 +15886,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="196" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>59</v>
       </c>
@@ -15874,7 +15918,7 @@
         <v>96</v>
       </c>
       <c r="N196" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O196" s="3" t="s">
         <v>86</v>
@@ -15910,7 +15954,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>198</v>
       </c>
@@ -15942,7 +15986,7 @@
         <v>96</v>
       </c>
       <c r="N197" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O197" s="3" t="s">
         <v>86</v>
@@ -15978,7 +16022,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="198" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>63</v>
       </c>
@@ -16010,7 +16054,7 @@
         <v>96</v>
       </c>
       <c r="N198" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O198" s="3" t="s">
         <v>86</v>
@@ -16046,7 +16090,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="199" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>199</v>
       </c>
@@ -16078,7 +16122,7 @@
         <v>96</v>
       </c>
       <c r="N199" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O199" s="3" t="s">
         <v>86</v>
@@ -16114,7 +16158,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="200" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
         <v>200</v>
       </c>
@@ -16146,7 +16190,7 @@
         <v>96</v>
       </c>
       <c r="N200" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O200" s="3" t="s">
         <v>86</v>
@@ -16182,7 +16226,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="201" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
         <v>201</v>
       </c>
@@ -16214,7 +16258,7 @@
         <v>96</v>
       </c>
       <c r="N201" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O201" s="3" t="s">
         <v>86</v>
@@ -16250,7 +16294,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="202" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>202</v>
       </c>
@@ -16282,7 +16326,7 @@
         <v>76</v>
       </c>
       <c r="N202" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O202" s="6" t="s">
         <v>81</v>
@@ -16318,7 +16362,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="203" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>203</v>
       </c>
@@ -16350,7 +16394,7 @@
         <v>76</v>
       </c>
       <c r="N203" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O203" s="6" t="s">
         <v>81</v>
@@ -16386,7 +16430,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="204" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>118</v>
       </c>
@@ -16418,7 +16462,7 @@
         <v>76</v>
       </c>
       <c r="N204" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O204" s="6" t="s">
         <v>81</v>
@@ -16454,7 +16498,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="205" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>204</v>
       </c>
@@ -16486,7 +16530,7 @@
         <v>76</v>
       </c>
       <c r="N205" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O205" s="6" t="s">
         <v>81</v>
@@ -16522,7 +16566,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="206" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
         <v>205</v>
       </c>
@@ -16554,7 +16598,7 @@
         <v>76</v>
       </c>
       <c r="N206" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O206" s="6" t="s">
         <v>81</v>
@@ -16590,7 +16634,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="207" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>206</v>
       </c>
@@ -16622,7 +16666,7 @@
         <v>76</v>
       </c>
       <c r="N207" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O207" s="6" t="s">
         <v>81</v>
@@ -16658,7 +16702,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="208" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>127</v>
       </c>
@@ -16690,7 +16734,7 @@
         <v>76</v>
       </c>
       <c r="N208" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O208" s="6" t="s">
         <v>81</v>
@@ -16726,7 +16770,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="209" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
         <v>128</v>
       </c>
@@ -16758,7 +16802,7 @@
         <v>76</v>
       </c>
       <c r="N209" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O209" s="6" t="s">
         <v>81</v>
@@ -16794,7 +16838,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="210" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
         <v>129</v>
       </c>
@@ -16826,7 +16870,7 @@
         <v>76</v>
       </c>
       <c r="N210" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O210" s="6" t="s">
         <v>81</v>
@@ -16862,7 +16906,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>207</v>
       </c>
@@ -16894,7 +16938,7 @@
         <v>76</v>
       </c>
       <c r="N211" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O211" s="6" t="s">
         <v>81</v>
@@ -16930,7 +16974,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="212" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>208</v>
       </c>
@@ -16962,7 +17006,7 @@
         <v>76</v>
       </c>
       <c r="N212" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O212" s="6" t="s">
         <v>81</v>
@@ -16998,7 +17042,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="213" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
         <v>209</v>
       </c>
@@ -17030,7 +17074,7 @@
         <v>76</v>
       </c>
       <c r="N213" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O213" s="6" t="s">
         <v>81</v>
@@ -17066,7 +17110,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="214" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
         <v>179</v>
       </c>
@@ -17098,7 +17142,7 @@
         <v>76</v>
       </c>
       <c r="N214" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O214" s="6" t="s">
         <v>81</v>
@@ -17134,7 +17178,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="215" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
         <v>32</v>
       </c>
@@ -17166,7 +17210,7 @@
         <v>76</v>
       </c>
       <c r="N215" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O215" s="6" t="s">
         <v>81</v>
@@ -17202,7 +17246,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="216" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
         <v>210</v>
       </c>
@@ -17234,7 +17278,7 @@
         <v>76</v>
       </c>
       <c r="N216" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O216" s="6" t="s">
         <v>81</v>
@@ -17270,7 +17314,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="217" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
         <v>540</v>
       </c>
@@ -17305,7 +17349,7 @@
         <v>80</v>
       </c>
       <c r="N217" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O217" s="3" t="s">
         <v>81</v>
@@ -17341,7 +17385,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="218" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
         <v>542</v>
       </c>
@@ -17376,7 +17420,7 @@
         <v>80</v>
       </c>
       <c r="N218" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O218" s="3" t="s">
         <v>81</v>
@@ -17412,7 +17456,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>544</v>
       </c>
@@ -17447,7 +17491,7 @@
         <v>80</v>
       </c>
       <c r="N219" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O219" s="3" t="s">
         <v>81</v>
@@ -17483,7 +17527,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="220" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
         <v>546</v>
       </c>
@@ -17518,7 +17562,7 @@
         <v>80</v>
       </c>
       <c r="N220" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O220" s="3" t="s">
         <v>81</v>
@@ -17554,7 +17598,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="221" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>548</v>
       </c>
@@ -17589,7 +17633,7 @@
         <v>80</v>
       </c>
       <c r="N221" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O221" s="3" t="s">
         <v>81</v>
@@ -17625,7 +17669,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="222" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
         <v>550</v>
       </c>
@@ -17660,7 +17704,7 @@
         <v>80</v>
       </c>
       <c r="N222" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O222" s="3" t="s">
         <v>81</v>
@@ -17696,7 +17740,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="223" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
         <v>552</v>
       </c>
@@ -17731,7 +17775,7 @@
         <v>80</v>
       </c>
       <c r="N223" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O223" s="3" t="s">
         <v>81</v>
@@ -17767,7 +17811,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
         <v>554</v>
       </c>
@@ -17802,7 +17846,7 @@
         <v>80</v>
       </c>
       <c r="N224" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O224" s="3" t="s">
         <v>81</v>
@@ -17838,7 +17882,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="225" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>556</v>
       </c>
@@ -17873,7 +17917,7 @@
         <v>80</v>
       </c>
       <c r="N225" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O225" s="3" t="s">
         <v>81</v>
@@ -17909,7 +17953,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
         <v>558</v>
       </c>
@@ -17944,7 +17988,7 @@
         <v>80</v>
       </c>
       <c r="N226" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O226" s="3" t="s">
         <v>81</v>
@@ -17980,7 +18024,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="227" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>560</v>
       </c>
@@ -18015,7 +18059,7 @@
         <v>80</v>
       </c>
       <c r="N227" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O227" s="3" t="s">
         <v>81</v>
@@ -18051,7 +18095,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="228" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
         <v>562</v>
       </c>
@@ -18086,7 +18130,7 @@
         <v>80</v>
       </c>
       <c r="N228" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O228" s="3" t="s">
         <v>81</v>
@@ -18122,7 +18166,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="229" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>564</v>
       </c>
@@ -18157,7 +18201,7 @@
         <v>80</v>
       </c>
       <c r="N229" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O229" s="3" t="s">
         <v>81</v>
@@ -18194,7 +18238,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y229"/>
+  <autoFilter ref="A1:Y229" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new script for concept figure
</commit_message>
<xml_diff>
--- a/data/growth_data.xlsx
+++ b/data/growth_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48063D80-4BAB-E04B-8642-C340A0019301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A20E70-9D10-9E46-A69C-AD97954A8298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="33880" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4320" yWindow="460" windowWidth="29800" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -2269,9 +2269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V62" sqref="V62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7019,10 +7019,10 @@
         <v>9</v>
       </c>
       <c r="U66" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V66" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="V66" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="W66" s="4" t="s">
         <v>589</v>
@@ -7089,10 +7089,10 @@
         <v>9</v>
       </c>
       <c r="U67" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V67" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="V67" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="W67" s="4" t="s">
         <v>589</v>
@@ -7157,10 +7157,10 @@
         <v>9</v>
       </c>
       <c r="U68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V68" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="V68" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="W68" s="4" t="s">
         <v>589</v>
@@ -7225,10 +7225,10 @@
         <v>9</v>
       </c>
       <c r="U69" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V69" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="V69" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="W69" s="4" t="s">
         <v>589</v>
@@ -7293,10 +7293,10 @@
         <v>9</v>
       </c>
       <c r="U70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V70" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="V70" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="W70" s="4" t="s">
         <v>589</v>
@@ -7361,10 +7361,10 @@
         <v>9</v>
       </c>
       <c r="U71" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V71" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="V71" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="W71" s="4" t="s">
         <v>589</v>
@@ -7429,10 +7429,10 @@
         <v>9</v>
       </c>
       <c r="U72" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V72" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="V72" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="W72" s="4" t="s">
         <v>589</v>
@@ -7497,10 +7497,10 @@
         <v>9</v>
       </c>
       <c r="U73" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V73" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="V73" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="W73" s="4" t="s">
         <v>589</v>

</xml_diff>

<commit_message>
major update exploratroy analysis script, redoing figures
</commit_message>
<xml_diff>
--- a/data/growth_data.xlsx
+++ b/data/growth_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB3B3BC-730C-4F4F-9ECB-51920DC9C874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391B59E5-F8C6-E14E-83D1-E2550A28B66E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="460" windowWidth="35640" windowHeight="22360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,9 +902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA207" sqref="AA207"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10467,7 +10467,7 @@
       </c>
       <c r="C137" s="11"/>
       <c r="D137" s="11"/>
-      <c r="E137" s="12">
+      <c r="F137" s="12">
         <v>1.7</v>
       </c>
       <c r="G137" s="10" t="s">
@@ -10532,7 +10532,7 @@
       </c>
       <c r="C138" s="11"/>
       <c r="D138" s="11"/>
-      <c r="E138" s="12">
+      <c r="F138" s="12">
         <v>1.7</v>
       </c>
       <c r="G138" s="10" t="s">
@@ -10597,7 +10597,7 @@
       </c>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
-      <c r="E139" s="12">
+      <c r="F139" s="12">
         <v>1.7</v>
       </c>
       <c r="G139" s="10" t="s">
@@ -10662,7 +10662,7 @@
       </c>
       <c r="C140" s="11"/>
       <c r="D140" s="11"/>
-      <c r="E140" s="12">
+      <c r="F140" s="12">
         <v>1.7</v>
       </c>
       <c r="G140" s="10" t="s">
@@ -10727,7 +10727,7 @@
       </c>
       <c r="C141" s="11"/>
       <c r="D141" s="11"/>
-      <c r="E141" s="12">
+      <c r="F141" s="12">
         <v>1.7</v>
       </c>
       <c r="G141" s="10" t="s">
@@ -10792,7 +10792,7 @@
       </c>
       <c r="C142" s="11"/>
       <c r="D142" s="11"/>
-      <c r="E142" s="12">
+      <c r="F142" s="12">
         <v>1.7</v>
       </c>
       <c r="G142" s="10" t="s">
@@ -10857,7 +10857,7 @@
       </c>
       <c r="C143" s="11"/>
       <c r="D143" s="11"/>
-      <c r="E143" s="12">
+      <c r="F143" s="12">
         <v>1.9</v>
       </c>
       <c r="G143" s="10" t="s">
@@ -10922,7 +10922,7 @@
       </c>
       <c r="C144" s="11"/>
       <c r="D144" s="11"/>
-      <c r="E144" s="12">
+      <c r="F144" s="12">
         <v>1.9</v>
       </c>
       <c r="G144" s="10" t="s">
@@ -10987,7 +10987,7 @@
       </c>
       <c r="C145" s="11"/>
       <c r="D145" s="11"/>
-      <c r="E145" s="12">
+      <c r="F145" s="12">
         <v>1.9</v>
       </c>
       <c r="G145" s="10" t="s">
@@ -11052,7 +11052,7 @@
       </c>
       <c r="C146" s="11"/>
       <c r="D146" s="11"/>
-      <c r="E146" s="12">
+      <c r="F146" s="12">
         <v>1.9</v>
       </c>
       <c r="G146" s="10" t="s">
@@ -11117,7 +11117,7 @@
       </c>
       <c r="C147" s="11"/>
       <c r="D147" s="11"/>
-      <c r="E147" s="12">
+      <c r="F147" s="12">
         <v>1.9</v>
       </c>
       <c r="G147" s="10" t="s">
@@ -11182,7 +11182,7 @@
       </c>
       <c r="C148" s="11"/>
       <c r="D148" s="11"/>
-      <c r="E148" s="12">
+      <c r="F148" s="12">
         <v>1.9</v>
       </c>
       <c r="G148" s="10" t="s">
@@ -11247,7 +11247,7 @@
       </c>
       <c r="C149" s="11"/>
       <c r="D149" s="11"/>
-      <c r="E149" s="12">
+      <c r="F149" s="12">
         <v>4.4000000000000004</v>
       </c>
       <c r="G149" s="10" t="s">
@@ -11312,7 +11312,7 @@
       </c>
       <c r="C150" s="11"/>
       <c r="D150" s="11"/>
-      <c r="E150" s="12">
+      <c r="F150" s="12">
         <v>4.4000000000000004</v>
       </c>
       <c r="G150" s="10" t="s">
@@ -11377,7 +11377,7 @@
       </c>
       <c r="C151" s="11"/>
       <c r="D151" s="11"/>
-      <c r="E151" s="12">
+      <c r="F151" s="12">
         <v>4.4000000000000004</v>
       </c>
       <c r="G151" s="10" t="s">
@@ -11442,7 +11442,7 @@
       </c>
       <c r="C152" s="11"/>
       <c r="D152" s="11"/>
-      <c r="E152" s="12">
+      <c r="F152" s="12">
         <v>4.4000000000000004</v>
       </c>
       <c r="G152" s="10" t="s">
@@ -11507,7 +11507,7 @@
       </c>
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
-      <c r="E153" s="12">
+      <c r="F153" s="12">
         <v>4.4000000000000004</v>
       </c>
       <c r="G153" s="10" t="s">
@@ -11572,7 +11572,7 @@
       </c>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
-      <c r="E154" s="12">
+      <c r="F154" s="12">
         <v>13.7</v>
       </c>
       <c r="G154" s="10" t="s">
@@ -11637,7 +11637,7 @@
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
-      <c r="E155" s="12">
+      <c r="F155" s="12">
         <v>13.7</v>
       </c>
       <c r="G155" s="10" t="s">
@@ -11702,7 +11702,7 @@
       </c>
       <c r="C156" s="11"/>
       <c r="D156" s="11"/>
-      <c r="E156" s="12">
+      <c r="F156" s="12">
         <v>13.7</v>
       </c>
       <c r="G156" s="10" t="s">
@@ -11767,7 +11767,7 @@
       </c>
       <c r="C157" s="11"/>
       <c r="D157" s="11"/>
-      <c r="E157" s="12">
+      <c r="F157" s="12">
         <v>13.7</v>
       </c>
       <c r="G157" s="10" t="s">
@@ -11832,7 +11832,7 @@
       </c>
       <c r="C158" s="11"/>
       <c r="D158" s="11"/>
-      <c r="E158" s="12">
+      <c r="F158" s="12">
         <v>13.7</v>
       </c>
       <c r="G158" s="10" t="s">
@@ -11897,7 +11897,7 @@
       </c>
       <c r="C159" s="11"/>
       <c r="D159" s="11"/>
-      <c r="E159" s="12">
+      <c r="F159" s="12">
         <v>13.7</v>
       </c>
       <c r="G159" s="10" t="s">
@@ -11962,7 +11962,7 @@
       </c>
       <c r="C160" s="11"/>
       <c r="D160" s="11"/>
-      <c r="E160" s="12">
+      <c r="F160" s="12">
         <v>54</v>
       </c>
       <c r="G160" s="10" t="s">
@@ -12027,7 +12027,7 @@
       </c>
       <c r="C161" s="11"/>
       <c r="D161" s="11"/>
-      <c r="E161" s="12">
+      <c r="F161" s="12">
         <v>54</v>
       </c>
       <c r="G161" s="10" t="s">
@@ -12092,7 +12092,7 @@
       </c>
       <c r="C162" s="11"/>
       <c r="D162" s="11"/>
-      <c r="E162" s="12">
+      <c r="F162" s="12">
         <v>54</v>
       </c>
       <c r="G162" s="10" t="s">
@@ -12157,7 +12157,7 @@
       </c>
       <c r="C163" s="11"/>
       <c r="D163" s="11"/>
-      <c r="E163" s="12">
+      <c r="F163" s="12">
         <v>54</v>
       </c>
       <c r="G163" s="10" t="s">
@@ -12222,7 +12222,7 @@
       </c>
       <c r="C164" s="11"/>
       <c r="D164" s="11"/>
-      <c r="E164" s="12">
+      <c r="F164" s="12">
         <v>54</v>
       </c>
       <c r="G164" s="10" t="s">
@@ -12287,7 +12287,7 @@
       </c>
       <c r="C165" s="11"/>
       <c r="D165" s="11"/>
-      <c r="E165" s="12">
+      <c r="F165" s="12">
         <v>54</v>
       </c>
       <c r="G165" s="10" t="s">
@@ -12352,7 +12352,7 @@
       </c>
       <c r="C166" s="11"/>
       <c r="D166" s="11"/>
-      <c r="E166" s="12">
+      <c r="F166" s="12">
         <v>499</v>
       </c>
       <c r="G166" s="10" t="s">
@@ -12417,7 +12417,7 @@
       </c>
       <c r="C167" s="11"/>
       <c r="D167" s="11"/>
-      <c r="E167" s="12">
+      <c r="F167" s="12">
         <v>499</v>
       </c>
       <c r="G167" s="10" t="s">
@@ -12482,7 +12482,7 @@
       </c>
       <c r="C168" s="11"/>
       <c r="D168" s="11"/>
-      <c r="E168" s="12">
+      <c r="F168" s="12">
         <v>499</v>
       </c>
       <c r="G168" s="10" t="s">
@@ -12547,7 +12547,7 @@
       </c>
       <c r="C169" s="11"/>
       <c r="D169" s="11"/>
-      <c r="E169" s="12">
+      <c r="F169" s="12">
         <v>499</v>
       </c>
       <c r="G169" s="10" t="s">
@@ -12612,7 +12612,7 @@
       </c>
       <c r="C170" s="11"/>
       <c r="D170" s="11"/>
-      <c r="E170" s="12">
+      <c r="F170" s="12">
         <v>499</v>
       </c>
       <c r="G170" s="10" t="s">
@@ -12677,7 +12677,7 @@
       </c>
       <c r="C171" s="11"/>
       <c r="D171" s="11"/>
-      <c r="E171" s="12">
+      <c r="F171" s="12">
         <v>499</v>
       </c>
       <c r="G171" s="10" t="s">

</xml_diff>

<commit_message>
Added environemtn vs experiment temperature plot
</commit_message>
<xml_diff>
--- a/data/growth_data.xlsx
+++ b/data/growth_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391B59E5-F8C6-E14E-83D1-E2550A28B66E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA825FE-F352-3B40-A66C-80AE9ED84EA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="460" windowWidth="35640" windowHeight="22360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,9 +902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E142" sqref="E142"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
minor edits & cleanup before submission
</commit_message>
<xml_diff>
--- a/data/growth_data.xlsx
+++ b/data/growth_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A748F78B-B9C1-4244-BF7E-E27F7F9284F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AA2429-55B4-3D46-AFB3-867B12AF0FE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6200" yWindow="2340" windowWidth="29000" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29220" yWindow="3200" windowWidth="21200" windowHeight="12740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -366,9 +366,6 @@
     <t>Fish sizes are "about" the size specified; Weight at maturation based on median lengths from two fishbase sources; Optimum is temperature treatment yielding highest growth (not estimated)</t>
   </si>
   <si>
-    <t>Fish sizes are "about" the size specified; Weight at maturation based on min size of maturation (midpoint of sexes) from Cao etal 2009 Environ Biol Fish; Optimum is temperature treatment yielding highest growth (not estimated); Found through consumption search</t>
-  </si>
-  <si>
     <t>Only size classes with optimum presented here; Geometric mean from size window; Maturation size from preprint: https://doi.org/10.1101/382155</t>
   </si>
   <si>
@@ -454,6 +451,9 @@
   </si>
   <si>
     <t>Calculated sizes from mean TL using equation in Fig. 2; Multiple data points per temp and size, calculated mean in separate doc; w_maturation from Craig et al 1981 CJFA, age at maturatity 2,3, used geometric mean of length at age.</t>
+  </si>
+  <si>
+    <t>Weight at maturation based on min size of maturation (midpoint of sexes) from Cao etal 2009 Environ Biol Fish; Optimum is temperature treatment yielding highest growth (not estimated); Found through consumption search</t>
   </si>
 </sst>
 </file>
@@ -931,9 +931,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W228" sqref="W228"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W216" sqref="W216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -985,7 +985,7 @@
         <v>95</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1101,7 +1101,7 @@
         <v>13.5</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X2" s="10" t="s">
         <v>106</v>
@@ -1169,7 +1169,7 @@
         <v>13.5</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X3" s="10" t="s">
         <v>106</v>
@@ -1237,7 +1237,7 @@
         <v>13.5</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X4" s="10" t="s">
         <v>106</v>
@@ -1305,7 +1305,7 @@
         <v>13.5</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X5" s="10" t="s">
         <v>106</v>
@@ -1373,7 +1373,7 @@
         <v>13.5</v>
       </c>
       <c r="W6" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X6" s="10" t="s">
         <v>106</v>
@@ -1441,7 +1441,7 @@
         <v>13.5</v>
       </c>
       <c r="W7" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X7" s="10" t="s">
         <v>106</v>
@@ -1509,7 +1509,7 @@
         <v>13.5</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X8" s="10" t="s">
         <v>106</v>
@@ -1577,7 +1577,7 @@
         <v>13.5</v>
       </c>
       <c r="W9" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X9" s="10" t="s">
         <v>106</v>
@@ -1645,7 +1645,7 @@
         <v>13.5</v>
       </c>
       <c r="W10" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X10" s="10" t="s">
         <v>106</v>
@@ -1713,7 +1713,7 @@
         <v>13.5</v>
       </c>
       <c r="W11" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X11" s="10" t="s">
         <v>106</v>
@@ -1781,7 +1781,7 @@
         <v>13.5</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X12" s="10" t="s">
         <v>106</v>
@@ -1849,7 +1849,7 @@
         <v>13.5</v>
       </c>
       <c r="W13" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X13" s="10" t="s">
         <v>106</v>
@@ -1917,7 +1917,7 @@
         <v>13.5</v>
       </c>
       <c r="W14" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X14" s="10" t="s">
         <v>106</v>
@@ -1985,7 +1985,7 @@
         <v>13.5</v>
       </c>
       <c r="W15" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X15" s="10" t="s">
         <v>106</v>
@@ -2053,7 +2053,7 @@
         <v>13.5</v>
       </c>
       <c r="W16" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X16" s="10" t="s">
         <v>106</v>
@@ -2121,7 +2121,7 @@
         <v>13.5</v>
       </c>
       <c r="W17" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X17" s="10" t="s">
         <v>106</v>
@@ -2189,7 +2189,7 @@
         <v>13.5</v>
       </c>
       <c r="W18" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X18" s="10" t="s">
         <v>106</v>
@@ -2257,7 +2257,7 @@
         <v>13.5</v>
       </c>
       <c r="W19" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X19" s="10" t="s">
         <v>106</v>
@@ -2325,7 +2325,7 @@
         <v>6</v>
       </c>
       <c r="W20" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X20" s="10" t="s">
         <v>19</v>
@@ -2393,7 +2393,7 @@
         <v>6</v>
       </c>
       <c r="W21" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="X21" s="10" t="s">
         <v>19</v>
@@ -2461,7 +2461,7 @@
         <v>6</v>
       </c>
       <c r="W22" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="X22" s="10" t="s">
         <v>19</v>
@@ -2529,7 +2529,7 @@
         <v>6</v>
       </c>
       <c r="W23" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X23" s="10" t="s">
         <v>19</v>
@@ -2597,7 +2597,7 @@
         <v>6</v>
       </c>
       <c r="W24" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="X24" s="10" t="s">
         <v>19</v>
@@ -2665,7 +2665,7 @@
         <v>6</v>
       </c>
       <c r="W25" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X25" s="10" t="s">
         <v>19</v>
@@ -2733,7 +2733,7 @@
         <v>6</v>
       </c>
       <c r="W26" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="X26" s="10" t="s">
         <v>19</v>
@@ -2801,7 +2801,7 @@
         <v>6</v>
       </c>
       <c r="W27" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X27" s="10" t="s">
         <v>19</v>
@@ -2869,7 +2869,7 @@
         <v>6</v>
       </c>
       <c r="W28" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X28" s="10" t="s">
         <v>19</v>
@@ -2937,7 +2937,7 @@
         <v>6</v>
       </c>
       <c r="W29" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X29" s="10" t="s">
         <v>19</v>
@@ -3005,7 +3005,7 @@
         <v>6</v>
       </c>
       <c r="W30" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="X30" s="10" t="s">
         <v>19</v>
@@ -3073,7 +3073,7 @@
         <v>6</v>
       </c>
       <c r="W31" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="X31" s="10" t="s">
         <v>19</v>
@@ -3141,7 +3141,7 @@
         <v>6</v>
       </c>
       <c r="W32" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="X32" s="10" t="s">
         <v>19</v>
@@ -3209,7 +3209,7 @@
         <v>6</v>
       </c>
       <c r="W33" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X33" s="10" t="s">
         <v>19</v>
@@ -3277,7 +3277,7 @@
         <v>6</v>
       </c>
       <c r="W34" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="X34" s="10" t="s">
         <v>19</v>
@@ -3345,7 +3345,7 @@
         <v>6</v>
       </c>
       <c r="W35" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="X35" s="10" t="s">
         <v>19</v>
@@ -3413,7 +3413,7 @@
         <v>6</v>
       </c>
       <c r="W36" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="X36" s="10" t="s">
         <v>19</v>
@@ -3481,7 +3481,7 @@
         <v>6</v>
       </c>
       <c r="W37" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X37" s="10" t="s">
         <v>19</v>
@@ -3549,7 +3549,7 @@
         <v>6</v>
       </c>
       <c r="W38" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X38" s="10" t="s">
         <v>19</v>
@@ -3617,7 +3617,7 @@
         <v>6</v>
       </c>
       <c r="W39" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X39" s="10" t="s">
         <v>19</v>
@@ -5125,7 +5125,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W60" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X60" s="15" t="s">
         <v>25</v>
@@ -5193,7 +5193,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W61" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X61" s="15" t="s">
         <v>25</v>
@@ -5261,7 +5261,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W62" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X62" s="15" t="s">
         <v>25</v>
@@ -5329,7 +5329,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W63" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X63" s="15" t="s">
         <v>25</v>
@@ -5397,7 +5397,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W64" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X64" s="15" t="s">
         <v>25</v>
@@ -5465,7 +5465,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W65" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X65" s="15" t="s">
         <v>25</v>
@@ -5533,7 +5533,7 @@
         <v>8.4</v>
       </c>
       <c r="W66" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X66" s="15" t="s">
         <v>30</v>
@@ -5601,7 +5601,7 @@
         <v>8.4</v>
       </c>
       <c r="W67" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X67" s="15" t="s">
         <v>30</v>
@@ -5669,7 +5669,7 @@
         <v>8.4</v>
       </c>
       <c r="W68" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X68" s="15" t="s">
         <v>30</v>
@@ -5737,7 +5737,7 @@
         <v>8.4</v>
       </c>
       <c r="W69" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X69" s="15" t="s">
         <v>30</v>
@@ -5805,7 +5805,7 @@
         <v>8.4</v>
       </c>
       <c r="W70" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X70" s="15" t="s">
         <v>30</v>
@@ -5873,7 +5873,7 @@
         <v>8.4</v>
       </c>
       <c r="W71" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X71" s="15" t="s">
         <v>30</v>
@@ -5941,7 +5941,7 @@
         <v>8.4</v>
       </c>
       <c r="W72" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X72" s="15" t="s">
         <v>30</v>
@@ -6009,7 +6009,7 @@
         <v>8.4</v>
       </c>
       <c r="W73" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X73" s="15" t="s">
         <v>30</v>
@@ -9257,7 +9257,7 @@
         <v>4.2</v>
       </c>
       <c r="W120" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X120" s="10" t="s">
         <v>34</v>
@@ -9329,7 +9329,7 @@
         <v>4.2</v>
       </c>
       <c r="W121" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X121" s="10" t="s">
         <v>34</v>
@@ -9401,7 +9401,7 @@
         <v>4.2</v>
       </c>
       <c r="W122" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X122" s="10" t="s">
         <v>34</v>
@@ -9473,7 +9473,7 @@
         <v>4.2</v>
       </c>
       <c r="W123" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X123" s="10" t="s">
         <v>34</v>
@@ -9545,7 +9545,7 @@
         <v>4.2</v>
       </c>
       <c r="W124" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X124" s="10" t="s">
         <v>34</v>
@@ -9617,7 +9617,7 @@
         <v>4.2</v>
       </c>
       <c r="W125" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X125" s="10" t="s">
         <v>34</v>
@@ -9689,7 +9689,7 @@
         <v>4.2</v>
       </c>
       <c r="W126" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X126" s="10" t="s">
         <v>34</v>
@@ -9761,7 +9761,7 @@
         <v>4.2</v>
       </c>
       <c r="W127" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X127" s="10" t="s">
         <v>34</v>
@@ -9833,7 +9833,7 @@
         <v>4.2</v>
       </c>
       <c r="W128" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X128" s="10" t="s">
         <v>34</v>
@@ -9905,7 +9905,7 @@
         <v>4.2</v>
       </c>
       <c r="W129" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X129" s="10" t="s">
         <v>34</v>
@@ -9977,7 +9977,7 @@
         <v>4.2</v>
       </c>
       <c r="W130" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X130" s="10" t="s">
         <v>34</v>
@@ -10049,7 +10049,7 @@
         <v>4.2</v>
       </c>
       <c r="W131" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X131" s="10" t="s">
         <v>34</v>
@@ -10121,7 +10121,7 @@
         <v>4.2</v>
       </c>
       <c r="W132" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X132" s="10" t="s">
         <v>34</v>
@@ -10193,7 +10193,7 @@
         <v>4.2</v>
       </c>
       <c r="W133" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X133" s="10" t="s">
         <v>34</v>
@@ -10265,7 +10265,7 @@
         <v>4.2</v>
       </c>
       <c r="W134" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X134" s="10" t="s">
         <v>34</v>
@@ -10337,7 +10337,7 @@
         <v>4.2</v>
       </c>
       <c r="W135" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X135" s="10" t="s">
         <v>34</v>
@@ -10409,7 +10409,7 @@
         <v>4.2</v>
       </c>
       <c r="W136" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X136" s="10" t="s">
         <v>34</v>
@@ -10476,7 +10476,7 @@
         <v>8.9</v>
       </c>
       <c r="W137" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X137" s="10" t="s">
         <v>37</v>
@@ -10543,7 +10543,7 @@
         <v>8.9</v>
       </c>
       <c r="W138" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X138" s="10" t="s">
         <v>37</v>
@@ -10610,7 +10610,7 @@
         <v>8.9</v>
       </c>
       <c r="W139" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X139" s="10" t="s">
         <v>37</v>
@@ -10677,7 +10677,7 @@
         <v>8.9</v>
       </c>
       <c r="W140" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X140" s="10" t="s">
         <v>37</v>
@@ -10744,7 +10744,7 @@
         <v>8.9</v>
       </c>
       <c r="W141" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X141" s="10" t="s">
         <v>37</v>
@@ -10811,7 +10811,7 @@
         <v>8.9</v>
       </c>
       <c r="W142" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X142" s="10" t="s">
         <v>37</v>
@@ -10878,7 +10878,7 @@
         <v>8.9</v>
       </c>
       <c r="W143" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X143" s="10" t="s">
         <v>37</v>
@@ -10945,7 +10945,7 @@
         <v>8.9</v>
       </c>
       <c r="W144" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X144" s="10" t="s">
         <v>37</v>
@@ -11012,7 +11012,7 @@
         <v>8.9</v>
       </c>
       <c r="W145" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X145" s="10" t="s">
         <v>37</v>
@@ -11079,7 +11079,7 @@
         <v>8.9</v>
       </c>
       <c r="W146" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X146" s="10" t="s">
         <v>37</v>
@@ -11146,7 +11146,7 @@
         <v>8.9</v>
       </c>
       <c r="W147" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X147" s="10" t="s">
         <v>37</v>
@@ -11213,7 +11213,7 @@
         <v>8.9</v>
       </c>
       <c r="W148" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X148" s="10" t="s">
         <v>37</v>
@@ -11280,7 +11280,7 @@
         <v>8.9</v>
       </c>
       <c r="W149" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X149" s="10" t="s">
         <v>37</v>
@@ -11347,7 +11347,7 @@
         <v>8.9</v>
       </c>
       <c r="W150" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X150" s="10" t="s">
         <v>37</v>
@@ -11414,7 +11414,7 @@
         <v>8.9</v>
       </c>
       <c r="W151" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X151" s="10" t="s">
         <v>37</v>
@@ -11481,7 +11481,7 @@
         <v>8.9</v>
       </c>
       <c r="W152" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X152" s="10" t="s">
         <v>37</v>
@@ -11548,7 +11548,7 @@
         <v>8.9</v>
       </c>
       <c r="W153" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X153" s="10" t="s">
         <v>37</v>
@@ -11615,7 +11615,7 @@
         <v>8.9</v>
       </c>
       <c r="W154" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X154" s="10" t="s">
         <v>37</v>
@@ -11682,7 +11682,7 @@
         <v>8.9</v>
       </c>
       <c r="W155" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X155" s="10" t="s">
         <v>37</v>
@@ -11749,7 +11749,7 @@
         <v>8.9</v>
       </c>
       <c r="W156" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X156" s="10" t="s">
         <v>37</v>
@@ -11816,7 +11816,7 @@
         <v>8.9</v>
       </c>
       <c r="W157" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X157" s="10" t="s">
         <v>37</v>
@@ -11883,7 +11883,7 @@
         <v>8.9</v>
       </c>
       <c r="W158" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X158" s="10" t="s">
         <v>37</v>
@@ -11950,7 +11950,7 @@
         <v>8.9</v>
       </c>
       <c r="W159" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X159" s="10" t="s">
         <v>37</v>
@@ -12017,7 +12017,7 @@
         <v>8.9</v>
       </c>
       <c r="W160" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X160" s="10" t="s">
         <v>37</v>
@@ -12084,7 +12084,7 @@
         <v>8.9</v>
       </c>
       <c r="W161" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X161" s="10" t="s">
         <v>37</v>
@@ -12151,7 +12151,7 @@
         <v>8.9</v>
       </c>
       <c r="W162" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X162" s="10" t="s">
         <v>37</v>
@@ -12218,7 +12218,7 @@
         <v>8.9</v>
       </c>
       <c r="W163" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X163" s="10" t="s">
         <v>37</v>
@@ -12285,7 +12285,7 @@
         <v>8.9</v>
       </c>
       <c r="W164" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X164" s="10" t="s">
         <v>37</v>
@@ -12352,7 +12352,7 @@
         <v>8.9</v>
       </c>
       <c r="W165" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X165" s="10" t="s">
         <v>37</v>
@@ -12419,7 +12419,7 @@
         <v>8.9</v>
       </c>
       <c r="W166" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X166" s="10" t="s">
         <v>37</v>
@@ -12486,7 +12486,7 @@
         <v>8.9</v>
       </c>
       <c r="W167" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X167" s="10" t="s">
         <v>37</v>
@@ -12553,7 +12553,7 @@
         <v>8.9</v>
       </c>
       <c r="W168" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X168" s="10" t="s">
         <v>37</v>
@@ -12620,7 +12620,7 @@
         <v>8.9</v>
       </c>
       <c r="W169" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X169" s="10" t="s">
         <v>37</v>
@@ -12687,7 +12687,7 @@
         <v>8.9</v>
       </c>
       <c r="W170" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X170" s="10" t="s">
         <v>37</v>
@@ -12754,7 +12754,7 @@
         <v>8.9</v>
       </c>
       <c r="W171" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X171" s="10" t="s">
         <v>37</v>
@@ -12822,7 +12822,7 @@
         <v>1.4</v>
       </c>
       <c r="W172" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X172" s="10" t="s">
         <v>43</v>
@@ -12890,7 +12890,7 @@
         <v>1.4</v>
       </c>
       <c r="W173" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X173" s="10" t="s">
         <v>43</v>
@@ -12958,7 +12958,7 @@
         <v>1.4</v>
       </c>
       <c r="W174" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X174" s="10" t="s">
         <v>43</v>
@@ -13026,7 +13026,7 @@
         <v>1.4</v>
       </c>
       <c r="W175" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X175" s="10" t="s">
         <v>43</v>
@@ -13094,7 +13094,7 @@
         <v>1.4</v>
       </c>
       <c r="W176" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X176" s="10" t="s">
         <v>43</v>
@@ -13162,7 +13162,7 @@
         <v>1.4</v>
       </c>
       <c r="W177" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X177" s="10" t="s">
         <v>43</v>
@@ -13230,7 +13230,7 @@
         <v>1.4</v>
       </c>
       <c r="W178" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X178" s="10" t="s">
         <v>43</v>
@@ -13298,7 +13298,7 @@
         <v>1.4</v>
       </c>
       <c r="W179" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X179" s="10" t="s">
         <v>43</v>
@@ -13366,7 +13366,7 @@
         <v>1.4</v>
       </c>
       <c r="W180" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X180" s="10" t="s">
         <v>43</v>
@@ -13434,7 +13434,7 @@
         <v>1.4</v>
       </c>
       <c r="W181" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X181" s="10" t="s">
         <v>43</v>
@@ -14862,10 +14862,10 @@
         <v>21</v>
       </c>
       <c r="W202" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X202" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="203" spans="1:24" x14ac:dyDescent="0.2">
@@ -14930,10 +14930,10 @@
         <v>21</v>
       </c>
       <c r="W203" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X203" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="204" spans="1:24" x14ac:dyDescent="0.2">
@@ -14998,10 +14998,10 @@
         <v>21</v>
       </c>
       <c r="W204" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X204" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="205" spans="1:24" x14ac:dyDescent="0.2">
@@ -15066,10 +15066,10 @@
         <v>21</v>
       </c>
       <c r="W205" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X205" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="206" spans="1:24" x14ac:dyDescent="0.2">
@@ -15134,10 +15134,10 @@
         <v>21</v>
       </c>
       <c r="W206" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X206" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="207" spans="1:24" x14ac:dyDescent="0.2">
@@ -15202,10 +15202,10 @@
         <v>21</v>
       </c>
       <c r="W207" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X207" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="208" spans="1:24" x14ac:dyDescent="0.2">
@@ -15270,10 +15270,10 @@
         <v>21</v>
       </c>
       <c r="W208" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X208" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="209" spans="1:24" x14ac:dyDescent="0.2">
@@ -15338,10 +15338,10 @@
         <v>21</v>
       </c>
       <c r="W209" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X209" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="210" spans="1:24" x14ac:dyDescent="0.2">
@@ -15406,10 +15406,10 @@
         <v>21</v>
       </c>
       <c r="W210" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X210" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="211" spans="1:24" x14ac:dyDescent="0.2">
@@ -15474,10 +15474,10 @@
         <v>21</v>
       </c>
       <c r="W211" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X211" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="212" spans="1:24" x14ac:dyDescent="0.2">
@@ -15542,10 +15542,10 @@
         <v>21</v>
       </c>
       <c r="W212" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X212" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="213" spans="1:24" x14ac:dyDescent="0.2">
@@ -15610,10 +15610,10 @@
         <v>21</v>
       </c>
       <c r="W213" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X213" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="214" spans="1:24" x14ac:dyDescent="0.2">
@@ -15678,10 +15678,10 @@
         <v>21</v>
       </c>
       <c r="W214" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X214" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="215" spans="1:24" x14ac:dyDescent="0.2">
@@ -15746,10 +15746,10 @@
         <v>21</v>
       </c>
       <c r="W215" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X215" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="216" spans="1:24" x14ac:dyDescent="0.2">
@@ -15814,10 +15814,10 @@
         <v>21</v>
       </c>
       <c r="W216" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="X216" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="217" spans="1:24" x14ac:dyDescent="0.2">
@@ -15882,7 +15882,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W217" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X217" s="10" t="s">
         <v>92</v>
@@ -15950,7 +15950,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W218" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X218" s="10" t="s">
         <v>92</v>
@@ -16018,7 +16018,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W219" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X219" s="10" t="s">
         <v>92</v>
@@ -16086,7 +16086,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W220" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X220" s="10" t="s">
         <v>92</v>
@@ -16154,7 +16154,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W221" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X221" s="10" t="s">
         <v>92</v>
@@ -16222,7 +16222,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W222" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X222" s="10" t="s">
         <v>92</v>
@@ -16290,7 +16290,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W223" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X223" s="10" t="s">
         <v>92</v>
@@ -16358,7 +16358,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W224" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X224" s="10" t="s">
         <v>92</v>
@@ -16426,7 +16426,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W225" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X225" s="10" t="s">
         <v>92</v>
@@ -16494,7 +16494,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W226" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X226" s="10" t="s">
         <v>92</v>
@@ -16562,7 +16562,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W227" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X227" s="10" t="s">
         <v>92</v>
@@ -16630,7 +16630,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W228" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X228" s="10" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
1st GCB revision, close to resubmission. Removed log-linear growth and polished text.
</commit_message>
<xml_diff>
--- a/data/growth_data.xlsx
+++ b/data/growth_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AA2429-55B4-3D46-AFB3-867B12AF0FE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58160B6-F529-E44C-A8DA-950995168FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29220" yWindow="3200" windowWidth="21200" windowHeight="12740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7880" yWindow="2460" windowWidth="29380" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -348,9 +348,6 @@
     <t>Reef-associated; oceanodromous</t>
   </si>
   <si>
-    <t>Tomiyama-etal-2018-J.Sea.Res</t>
-  </si>
-  <si>
     <t>Sizes are average initial and final; Maturation length 35 cm (mid male and female); Also goes by bastard halibut, Japaneese halibut or Olive flounder</t>
   </si>
   <si>
@@ -454,6 +451,9 @@
   </si>
   <si>
     <t>Weight at maturation based on min size of maturation (midpoint of sexes) from Cao etal 2009 Environ Biol Fish; Optimum is temperature treatment yielding highest growth (not estimated); Found through consumption search</t>
+  </si>
+  <si>
+    <t>Tomiyama-etal-2018-JSeaRes</t>
   </si>
 </sst>
 </file>
@@ -932,8 +932,8 @@
   <dimension ref="A1:X228"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W216" sqref="W216"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -967,7 +967,7 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>94</v>
@@ -985,7 +985,7 @@
         <v>95</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1101,10 +1101,10 @@
         <v>13.5</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
@@ -1169,10 +1169,10 @@
         <v>13.5</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -1237,10 +1237,10 @@
         <v>13.5</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1305,10 +1305,10 @@
         <v>13.5</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -1373,10 +1373,10 @@
         <v>13.5</v>
       </c>
       <c r="W6" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X6" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -1441,10 +1441,10 @@
         <v>13.5</v>
       </c>
       <c r="W7" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X7" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -1509,10 +1509,10 @@
         <v>13.5</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X8" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -1577,10 +1577,10 @@
         <v>13.5</v>
       </c>
       <c r="W9" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X9" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
@@ -1645,10 +1645,10 @@
         <v>13.5</v>
       </c>
       <c r="W10" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X10" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -1713,10 +1713,10 @@
         <v>13.5</v>
       </c>
       <c r="W11" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X11" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -1781,10 +1781,10 @@
         <v>13.5</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X12" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
@@ -1849,10 +1849,10 @@
         <v>13.5</v>
       </c>
       <c r="W13" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X13" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
@@ -1917,10 +1917,10 @@
         <v>13.5</v>
       </c>
       <c r="W14" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X14" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
@@ -1985,10 +1985,10 @@
         <v>13.5</v>
       </c>
       <c r="W15" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X15" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
@@ -2053,10 +2053,10 @@
         <v>13.5</v>
       </c>
       <c r="W16" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X16" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -2121,10 +2121,10 @@
         <v>13.5</v>
       </c>
       <c r="W17" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X17" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
@@ -2189,10 +2189,10 @@
         <v>13.5</v>
       </c>
       <c r="W18" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X18" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -2257,10 +2257,10 @@
         <v>13.5</v>
       </c>
       <c r="W19" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X19" s="10" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -2325,7 +2325,7 @@
         <v>6</v>
       </c>
       <c r="W20" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X20" s="10" t="s">
         <v>19</v>
@@ -2393,7 +2393,7 @@
         <v>6</v>
       </c>
       <c r="W21" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X21" s="10" t="s">
         <v>19</v>
@@ -2461,7 +2461,7 @@
         <v>6</v>
       </c>
       <c r="W22" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="X22" s="10" t="s">
         <v>19</v>
@@ -2529,7 +2529,7 @@
         <v>6</v>
       </c>
       <c r="W23" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="X23" s="10" t="s">
         <v>19</v>
@@ -2597,7 +2597,7 @@
         <v>6</v>
       </c>
       <c r="W24" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X24" s="10" t="s">
         <v>19</v>
@@ -2665,7 +2665,7 @@
         <v>6</v>
       </c>
       <c r="W25" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="X25" s="10" t="s">
         <v>19</v>
@@ -2733,7 +2733,7 @@
         <v>6</v>
       </c>
       <c r="W26" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X26" s="10" t="s">
         <v>19</v>
@@ -2801,7 +2801,7 @@
         <v>6</v>
       </c>
       <c r="W27" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="X27" s="10" t="s">
         <v>19</v>
@@ -2869,7 +2869,7 @@
         <v>6</v>
       </c>
       <c r="W28" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X28" s="10" t="s">
         <v>19</v>
@@ -2937,7 +2937,7 @@
         <v>6</v>
       </c>
       <c r="W29" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X29" s="10" t="s">
         <v>19</v>
@@ -3005,7 +3005,7 @@
         <v>6</v>
       </c>
       <c r="W30" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X30" s="10" t="s">
         <v>19</v>
@@ -3073,7 +3073,7 @@
         <v>6</v>
       </c>
       <c r="W31" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="X31" s="10" t="s">
         <v>19</v>
@@ -3141,7 +3141,7 @@
         <v>6</v>
       </c>
       <c r="W32" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="X32" s="10" t="s">
         <v>19</v>
@@ -3209,7 +3209,7 @@
         <v>6</v>
       </c>
       <c r="W33" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="X33" s="10" t="s">
         <v>19</v>
@@ -3277,7 +3277,7 @@
         <v>6</v>
       </c>
       <c r="W34" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X34" s="10" t="s">
         <v>19</v>
@@ -3345,7 +3345,7 @@
         <v>6</v>
       </c>
       <c r="W35" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="X35" s="10" t="s">
         <v>19</v>
@@ -3413,7 +3413,7 @@
         <v>6</v>
       </c>
       <c r="W36" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="X36" s="10" t="s">
         <v>19</v>
@@ -3481,7 +3481,7 @@
         <v>6</v>
       </c>
       <c r="W37" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="X37" s="10" t="s">
         <v>19</v>
@@ -3549,7 +3549,7 @@
         <v>6</v>
       </c>
       <c r="W38" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X38" s="10" t="s">
         <v>19</v>
@@ -3617,7 +3617,7 @@
         <v>6</v>
       </c>
       <c r="W39" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X39" s="10" t="s">
         <v>19</v>
@@ -3689,7 +3689,7 @@
         <v>16.8</v>
       </c>
       <c r="W40" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X40" s="10" t="s">
         <v>24</v>
@@ -3761,7 +3761,7 @@
         <v>16.8</v>
       </c>
       <c r="W41" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X41" s="10" t="s">
         <v>24</v>
@@ -3833,7 +3833,7 @@
         <v>16.8</v>
       </c>
       <c r="W42" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X42" s="10" t="s">
         <v>24</v>
@@ -3905,7 +3905,7 @@
         <v>16.8</v>
       </c>
       <c r="W43" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X43" s="10" t="s">
         <v>24</v>
@@ -3977,7 +3977,7 @@
         <v>16.8</v>
       </c>
       <c r="W44" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X44" s="10" t="s">
         <v>24</v>
@@ -4049,7 +4049,7 @@
         <v>16.8</v>
       </c>
       <c r="W45" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X45" s="10" t="s">
         <v>24</v>
@@ -4121,7 +4121,7 @@
         <v>16.8</v>
       </c>
       <c r="W46" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X46" s="10" t="s">
         <v>24</v>
@@ -4193,7 +4193,7 @@
         <v>16.8</v>
       </c>
       <c r="W47" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X47" s="10" t="s">
         <v>24</v>
@@ -4265,7 +4265,7 @@
         <v>16.8</v>
       </c>
       <c r="W48" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X48" s="10" t="s">
         <v>24</v>
@@ -4337,7 +4337,7 @@
         <v>16.8</v>
       </c>
       <c r="W49" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X49" s="10" t="s">
         <v>24</v>
@@ -4409,7 +4409,7 @@
         <v>16.8</v>
       </c>
       <c r="W50" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X50" s="10" t="s">
         <v>24</v>
@@ -4481,7 +4481,7 @@
         <v>16.8</v>
       </c>
       <c r="W51" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X51" s="10" t="s">
         <v>24</v>
@@ -4553,7 +4553,7 @@
         <v>16.8</v>
       </c>
       <c r="W52" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X52" s="10" t="s">
         <v>24</v>
@@ -4625,7 +4625,7 @@
         <v>16.8</v>
       </c>
       <c r="W53" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X53" s="10" t="s">
         <v>24</v>
@@ -4697,7 +4697,7 @@
         <v>16.8</v>
       </c>
       <c r="W54" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X54" s="10" t="s">
         <v>24</v>
@@ -4769,7 +4769,7 @@
         <v>16.8</v>
       </c>
       <c r="W55" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X55" s="10" t="s">
         <v>24</v>
@@ -4841,7 +4841,7 @@
         <v>16.8</v>
       </c>
       <c r="W56" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X56" s="10" t="s">
         <v>24</v>
@@ -4913,7 +4913,7 @@
         <v>16.8</v>
       </c>
       <c r="W57" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X57" s="10" t="s">
         <v>24</v>
@@ -4985,7 +4985,7 @@
         <v>16.8</v>
       </c>
       <c r="W58" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X58" s="10" t="s">
         <v>24</v>
@@ -5057,7 +5057,7 @@
         <v>16.8</v>
       </c>
       <c r="W59" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X59" s="10" t="s">
         <v>24</v>
@@ -5125,7 +5125,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W60" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X60" s="15" t="s">
         <v>25</v>
@@ -5193,7 +5193,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W61" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X61" s="15" t="s">
         <v>25</v>
@@ -5261,7 +5261,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W62" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X62" s="15" t="s">
         <v>25</v>
@@ -5329,7 +5329,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W63" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X63" s="15" t="s">
         <v>25</v>
@@ -5397,7 +5397,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W64" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X64" s="15" t="s">
         <v>25</v>
@@ -5465,7 +5465,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="W65" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X65" s="15" t="s">
         <v>25</v>
@@ -5533,7 +5533,7 @@
         <v>8.4</v>
       </c>
       <c r="W66" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X66" s="15" t="s">
         <v>30</v>
@@ -5601,7 +5601,7 @@
         <v>8.4</v>
       </c>
       <c r="W67" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X67" s="15" t="s">
         <v>30</v>
@@ -5669,7 +5669,7 @@
         <v>8.4</v>
       </c>
       <c r="W68" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X68" s="15" t="s">
         <v>30</v>
@@ -5737,7 +5737,7 @@
         <v>8.4</v>
       </c>
       <c r="W69" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X69" s="15" t="s">
         <v>30</v>
@@ -5805,7 +5805,7 @@
         <v>8.4</v>
       </c>
       <c r="W70" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X70" s="15" t="s">
         <v>30</v>
@@ -5873,7 +5873,7 @@
         <v>8.4</v>
       </c>
       <c r="W71" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X71" s="15" t="s">
         <v>30</v>
@@ -5941,7 +5941,7 @@
         <v>8.4</v>
       </c>
       <c r="W72" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X72" s="15" t="s">
         <v>30</v>
@@ -6009,7 +6009,7 @@
         <v>8.4</v>
       </c>
       <c r="W73" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X73" s="15" t="s">
         <v>30</v>
@@ -6081,7 +6081,7 @@
         <v>27.05</v>
       </c>
       <c r="W74" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X74" s="15" t="s">
         <v>93</v>
@@ -6153,7 +6153,7 @@
         <v>27.05</v>
       </c>
       <c r="W75" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X75" s="15" t="s">
         <v>93</v>
@@ -6225,7 +6225,7 @@
         <v>27.05</v>
       </c>
       <c r="W76" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X76" s="15" t="s">
         <v>93</v>
@@ -6297,7 +6297,7 @@
         <v>27.05</v>
       </c>
       <c r="W77" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X77" s="15" t="s">
         <v>93</v>
@@ -6369,7 +6369,7 @@
         <v>27.05</v>
       </c>
       <c r="W78" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X78" s="15" t="s">
         <v>93</v>
@@ -6441,7 +6441,7 @@
         <v>27.05</v>
       </c>
       <c r="W79" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X79" s="15" t="s">
         <v>93</v>
@@ -6513,7 +6513,7 @@
         <v>27.05</v>
       </c>
       <c r="W80" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X80" s="15" t="s">
         <v>93</v>
@@ -6585,7 +6585,7 @@
         <v>27.05</v>
       </c>
       <c r="W81" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X81" s="15" t="s">
         <v>93</v>
@@ -6657,7 +6657,7 @@
         <v>27.05</v>
       </c>
       <c r="W82" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X82" s="15" t="s">
         <v>93</v>
@@ -6729,7 +6729,7 @@
         <v>27.05</v>
       </c>
       <c r="W83" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X83" s="15" t="s">
         <v>93</v>
@@ -6801,7 +6801,7 @@
         <v>27.05</v>
       </c>
       <c r="W84" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X84" s="15" t="s">
         <v>93</v>
@@ -6873,7 +6873,7 @@
         <v>27.05</v>
       </c>
       <c r="W85" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X85" s="15" t="s">
         <v>93</v>
@@ -6941,7 +6941,7 @@
         <v>5.4</v>
       </c>
       <c r="W86" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X86" s="10" t="s">
         <v>89</v>
@@ -7009,7 +7009,7 @@
         <v>5.4</v>
       </c>
       <c r="W87" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X87" s="10" t="s">
         <v>89</v>
@@ -7077,7 +7077,7 @@
         <v>5.4</v>
       </c>
       <c r="W88" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X88" s="10" t="s">
         <v>89</v>
@@ -7145,7 +7145,7 @@
         <v>5.4</v>
       </c>
       <c r="W89" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X89" s="10" t="s">
         <v>89</v>
@@ -7213,7 +7213,7 @@
         <v>5.4</v>
       </c>
       <c r="W90" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X90" s="10" t="s">
         <v>89</v>
@@ -7281,7 +7281,7 @@
         <v>5.4</v>
       </c>
       <c r="W91" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X91" s="10" t="s">
         <v>89</v>
@@ -7349,7 +7349,7 @@
         <v>5.4</v>
       </c>
       <c r="W92" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X92" s="10" t="s">
         <v>89</v>
@@ -7417,7 +7417,7 @@
         <v>5.4</v>
       </c>
       <c r="W93" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X93" s="10" t="s">
         <v>89</v>
@@ -7485,7 +7485,7 @@
         <v>5.4</v>
       </c>
       <c r="W94" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X94" s="10" t="s">
         <v>89</v>
@@ -7553,7 +7553,7 @@
         <v>5.4</v>
       </c>
       <c r="W95" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X95" s="10" t="s">
         <v>89</v>
@@ -7621,7 +7621,7 @@
         <v>5.4</v>
       </c>
       <c r="W96" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X96" s="10" t="s">
         <v>89</v>
@@ -7689,7 +7689,7 @@
         <v>5.4</v>
       </c>
       <c r="W97" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X97" s="10" t="s">
         <v>89</v>
@@ -7757,7 +7757,7 @@
         <v>5.4</v>
       </c>
       <c r="W98" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X98" s="10" t="s">
         <v>89</v>
@@ -7825,7 +7825,7 @@
         <v>5.4</v>
       </c>
       <c r="W99" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X99" s="10" t="s">
         <v>89</v>
@@ -7893,7 +7893,7 @@
         <v>5.4</v>
       </c>
       <c r="W100" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X100" s="10" t="s">
         <v>89</v>
@@ -7961,7 +7961,7 @@
         <v>5.4</v>
       </c>
       <c r="W101" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X101" s="10" t="s">
         <v>89</v>
@@ -8029,7 +8029,7 @@
         <v>5.4</v>
       </c>
       <c r="W102" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X102" s="10" t="s">
         <v>89</v>
@@ -8097,7 +8097,7 @@
         <v>5.4</v>
       </c>
       <c r="W103" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X103" s="10" t="s">
         <v>89</v>
@@ -8165,7 +8165,7 @@
         <v>5.4</v>
       </c>
       <c r="W104" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X104" s="10" t="s">
         <v>89</v>
@@ -8233,7 +8233,7 @@
         <v>5.4</v>
       </c>
       <c r="W105" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X105" s="10" t="s">
         <v>89</v>
@@ -8301,7 +8301,7 @@
         <v>5.4</v>
       </c>
       <c r="W106" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X106" s="10" t="s">
         <v>89</v>
@@ -8369,7 +8369,7 @@
         <v>5.4</v>
       </c>
       <c r="W107" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X107" s="10" t="s">
         <v>89</v>
@@ -8437,7 +8437,7 @@
         <v>5.4</v>
       </c>
       <c r="W108" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X108" s="10" t="s">
         <v>89</v>
@@ -8505,7 +8505,7 @@
         <v>5.4</v>
       </c>
       <c r="W109" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X109" s="10" t="s">
         <v>89</v>
@@ -8573,7 +8573,7 @@
         <v>5.4</v>
       </c>
       <c r="W110" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X110" s="10" t="s">
         <v>89</v>
@@ -8641,7 +8641,7 @@
         <v>5.4</v>
       </c>
       <c r="W111" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X111" s="10" t="s">
         <v>89</v>
@@ -8709,7 +8709,7 @@
         <v>5.4</v>
       </c>
       <c r="W112" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X112" s="10" t="s">
         <v>89</v>
@@ -8777,7 +8777,7 @@
         <v>5.4</v>
       </c>
       <c r="W113" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X113" s="10" t="s">
         <v>89</v>
@@ -8845,7 +8845,7 @@
         <v>5.4</v>
       </c>
       <c r="W114" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X114" s="10" t="s">
         <v>89</v>
@@ -8913,7 +8913,7 @@
         <v>5.4</v>
       </c>
       <c r="W115" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X115" s="10" t="s">
         <v>89</v>
@@ -8981,7 +8981,7 @@
         <v>5.4</v>
       </c>
       <c r="W116" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X116" s="10" t="s">
         <v>89</v>
@@ -9049,7 +9049,7 @@
         <v>5.4</v>
       </c>
       <c r="W117" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X117" s="10" t="s">
         <v>89</v>
@@ -9117,7 +9117,7 @@
         <v>5.4</v>
       </c>
       <c r="W118" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X118" s="10" t="s">
         <v>89</v>
@@ -9185,7 +9185,7 @@
         <v>5.4</v>
       </c>
       <c r="W119" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X119" s="10" t="s">
         <v>89</v>
@@ -9257,7 +9257,7 @@
         <v>4.2</v>
       </c>
       <c r="W120" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X120" s="10" t="s">
         <v>34</v>
@@ -9329,7 +9329,7 @@
         <v>4.2</v>
       </c>
       <c r="W121" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X121" s="10" t="s">
         <v>34</v>
@@ -9401,7 +9401,7 @@
         <v>4.2</v>
       </c>
       <c r="W122" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X122" s="10" t="s">
         <v>34</v>
@@ -9473,7 +9473,7 @@
         <v>4.2</v>
       </c>
       <c r="W123" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X123" s="10" t="s">
         <v>34</v>
@@ -9545,7 +9545,7 @@
         <v>4.2</v>
       </c>
       <c r="W124" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X124" s="10" t="s">
         <v>34</v>
@@ -9617,7 +9617,7 @@
         <v>4.2</v>
       </c>
       <c r="W125" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X125" s="10" t="s">
         <v>34</v>
@@ -9689,7 +9689,7 @@
         <v>4.2</v>
       </c>
       <c r="W126" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X126" s="10" t="s">
         <v>34</v>
@@ -9761,7 +9761,7 @@
         <v>4.2</v>
       </c>
       <c r="W127" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X127" s="10" t="s">
         <v>34</v>
@@ -9833,7 +9833,7 @@
         <v>4.2</v>
       </c>
       <c r="W128" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X128" s="10" t="s">
         <v>34</v>
@@ -9905,7 +9905,7 @@
         <v>4.2</v>
       </c>
       <c r="W129" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X129" s="10" t="s">
         <v>34</v>
@@ -9977,7 +9977,7 @@
         <v>4.2</v>
       </c>
       <c r="W130" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X130" s="10" t="s">
         <v>34</v>
@@ -10049,7 +10049,7 @@
         <v>4.2</v>
       </c>
       <c r="W131" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X131" s="10" t="s">
         <v>34</v>
@@ -10121,7 +10121,7 @@
         <v>4.2</v>
       </c>
       <c r="W132" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X132" s="10" t="s">
         <v>34</v>
@@ -10193,7 +10193,7 @@
         <v>4.2</v>
       </c>
       <c r="W133" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X133" s="10" t="s">
         <v>34</v>
@@ -10265,7 +10265,7 @@
         <v>4.2</v>
       </c>
       <c r="W134" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X134" s="10" t="s">
         <v>34</v>
@@ -10337,7 +10337,7 @@
         <v>4.2</v>
       </c>
       <c r="W135" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X135" s="10" t="s">
         <v>34</v>
@@ -10409,7 +10409,7 @@
         <v>4.2</v>
       </c>
       <c r="W136" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X136" s="10" t="s">
         <v>34</v>
@@ -10476,7 +10476,7 @@
         <v>8.9</v>
       </c>
       <c r="W137" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X137" s="10" t="s">
         <v>37</v>
@@ -10543,7 +10543,7 @@
         <v>8.9</v>
       </c>
       <c r="W138" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X138" s="10" t="s">
         <v>37</v>
@@ -10610,7 +10610,7 @@
         <v>8.9</v>
       </c>
       <c r="W139" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X139" s="10" t="s">
         <v>37</v>
@@ -10677,7 +10677,7 @@
         <v>8.9</v>
       </c>
       <c r="W140" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X140" s="10" t="s">
         <v>37</v>
@@ -10744,7 +10744,7 @@
         <v>8.9</v>
       </c>
       <c r="W141" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X141" s="10" t="s">
         <v>37</v>
@@ -10811,7 +10811,7 @@
         <v>8.9</v>
       </c>
       <c r="W142" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X142" s="10" t="s">
         <v>37</v>
@@ -10878,7 +10878,7 @@
         <v>8.9</v>
       </c>
       <c r="W143" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X143" s="10" t="s">
         <v>37</v>
@@ -10945,7 +10945,7 @@
         <v>8.9</v>
       </c>
       <c r="W144" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X144" s="10" t="s">
         <v>37</v>
@@ -11012,7 +11012,7 @@
         <v>8.9</v>
       </c>
       <c r="W145" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X145" s="10" t="s">
         <v>37</v>
@@ -11079,7 +11079,7 @@
         <v>8.9</v>
       </c>
       <c r="W146" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X146" s="10" t="s">
         <v>37</v>
@@ -11146,7 +11146,7 @@
         <v>8.9</v>
       </c>
       <c r="W147" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X147" s="10" t="s">
         <v>37</v>
@@ -11213,7 +11213,7 @@
         <v>8.9</v>
       </c>
       <c r="W148" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X148" s="10" t="s">
         <v>37</v>
@@ -11280,7 +11280,7 @@
         <v>8.9</v>
       </c>
       <c r="W149" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X149" s="10" t="s">
         <v>37</v>
@@ -11347,7 +11347,7 @@
         <v>8.9</v>
       </c>
       <c r="W150" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X150" s="10" t="s">
         <v>37</v>
@@ -11414,7 +11414,7 @@
         <v>8.9</v>
       </c>
       <c r="W151" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X151" s="10" t="s">
         <v>37</v>
@@ -11481,7 +11481,7 @@
         <v>8.9</v>
       </c>
       <c r="W152" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X152" s="10" t="s">
         <v>37</v>
@@ -11548,7 +11548,7 @@
         <v>8.9</v>
       </c>
       <c r="W153" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X153" s="10" t="s">
         <v>37</v>
@@ -11615,7 +11615,7 @@
         <v>8.9</v>
       </c>
       <c r="W154" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X154" s="10" t="s">
         <v>37</v>
@@ -11682,7 +11682,7 @@
         <v>8.9</v>
       </c>
       <c r="W155" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X155" s="10" t="s">
         <v>37</v>
@@ -11749,7 +11749,7 @@
         <v>8.9</v>
       </c>
       <c r="W156" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X156" s="10" t="s">
         <v>37</v>
@@ -11816,7 +11816,7 @@
         <v>8.9</v>
       </c>
       <c r="W157" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X157" s="10" t="s">
         <v>37</v>
@@ -11883,7 +11883,7 @@
         <v>8.9</v>
       </c>
       <c r="W158" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X158" s="10" t="s">
         <v>37</v>
@@ -11950,7 +11950,7 @@
         <v>8.9</v>
       </c>
       <c r="W159" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X159" s="10" t="s">
         <v>37</v>
@@ -12017,7 +12017,7 @@
         <v>8.9</v>
       </c>
       <c r="W160" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X160" s="10" t="s">
         <v>37</v>
@@ -12084,7 +12084,7 @@
         <v>8.9</v>
       </c>
       <c r="W161" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X161" s="10" t="s">
         <v>37</v>
@@ -12151,7 +12151,7 @@
         <v>8.9</v>
       </c>
       <c r="W162" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X162" s="10" t="s">
         <v>37</v>
@@ -12218,7 +12218,7 @@
         <v>8.9</v>
       </c>
       <c r="W163" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X163" s="10" t="s">
         <v>37</v>
@@ -12285,7 +12285,7 @@
         <v>8.9</v>
       </c>
       <c r="W164" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X164" s="10" t="s">
         <v>37</v>
@@ -12352,7 +12352,7 @@
         <v>8.9</v>
       </c>
       <c r="W165" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X165" s="10" t="s">
         <v>37</v>
@@ -12419,7 +12419,7 @@
         <v>8.9</v>
       </c>
       <c r="W166" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X166" s="10" t="s">
         <v>37</v>
@@ -12486,7 +12486,7 @@
         <v>8.9</v>
       </c>
       <c r="W167" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X167" s="10" t="s">
         <v>37</v>
@@ -12553,7 +12553,7 @@
         <v>8.9</v>
       </c>
       <c r="W168" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X168" s="10" t="s">
         <v>37</v>
@@ -12620,7 +12620,7 @@
         <v>8.9</v>
       </c>
       <c r="W169" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X169" s="10" t="s">
         <v>37</v>
@@ -12687,7 +12687,7 @@
         <v>8.9</v>
       </c>
       <c r="W170" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X170" s="10" t="s">
         <v>37</v>
@@ -12754,7 +12754,7 @@
         <v>8.9</v>
       </c>
       <c r="W171" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X171" s="10" t="s">
         <v>37</v>
@@ -12822,7 +12822,7 @@
         <v>1.4</v>
       </c>
       <c r="W172" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X172" s="10" t="s">
         <v>43</v>
@@ -12890,7 +12890,7 @@
         <v>1.4</v>
       </c>
       <c r="W173" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X173" s="10" t="s">
         <v>43</v>
@@ -12958,7 +12958,7 @@
         <v>1.4</v>
       </c>
       <c r="W174" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X174" s="10" t="s">
         <v>43</v>
@@ -13026,7 +13026,7 @@
         <v>1.4</v>
       </c>
       <c r="W175" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X175" s="10" t="s">
         <v>43</v>
@@ -13094,7 +13094,7 @@
         <v>1.4</v>
       </c>
       <c r="W176" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X176" s="10" t="s">
         <v>43</v>
@@ -13162,7 +13162,7 @@
         <v>1.4</v>
       </c>
       <c r="W177" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X177" s="10" t="s">
         <v>43</v>
@@ -13230,7 +13230,7 @@
         <v>1.4</v>
       </c>
       <c r="W178" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X178" s="10" t="s">
         <v>43</v>
@@ -13298,7 +13298,7 @@
         <v>1.4</v>
       </c>
       <c r="W179" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X179" s="10" t="s">
         <v>43</v>
@@ -13366,7 +13366,7 @@
         <v>1.4</v>
       </c>
       <c r="W180" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X180" s="10" t="s">
         <v>43</v>
@@ -13434,7 +13434,7 @@
         <v>1.4</v>
       </c>
       <c r="W181" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X181" s="10" t="s">
         <v>43</v>
@@ -13502,7 +13502,7 @@
         <v>13.95</v>
       </c>
       <c r="W182" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X182" s="10" t="s">
         <v>46</v>
@@ -13570,7 +13570,7 @@
         <v>13.95</v>
       </c>
       <c r="W183" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X183" s="10" t="s">
         <v>46</v>
@@ -13638,7 +13638,7 @@
         <v>13.95</v>
       </c>
       <c r="W184" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X184" s="10" t="s">
         <v>46</v>
@@ -13706,7 +13706,7 @@
         <v>13.95</v>
       </c>
       <c r="W185" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X185" s="10" t="s">
         <v>46</v>
@@ -13774,7 +13774,7 @@
         <v>13.95</v>
       </c>
       <c r="W186" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X186" s="10" t="s">
         <v>46</v>
@@ -13842,7 +13842,7 @@
         <v>13.95</v>
       </c>
       <c r="W187" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X187" s="10" t="s">
         <v>46</v>
@@ -13910,7 +13910,7 @@
         <v>13.95</v>
       </c>
       <c r="W188" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X188" s="10" t="s">
         <v>46</v>
@@ -13978,7 +13978,7 @@
         <v>13.95</v>
       </c>
       <c r="W189" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X189" s="10" t="s">
         <v>46</v>
@@ -14046,7 +14046,7 @@
         <v>13.95</v>
       </c>
       <c r="W190" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X190" s="10" t="s">
         <v>46</v>
@@ -14114,7 +14114,7 @@
         <v>13.95</v>
       </c>
       <c r="W191" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X191" s="10" t="s">
         <v>46</v>
@@ -14182,7 +14182,7 @@
         <v>13.95</v>
       </c>
       <c r="W192" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X192" s="10" t="s">
         <v>46</v>
@@ -14250,7 +14250,7 @@
         <v>13.95</v>
       </c>
       <c r="W193" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X193" s="10" t="s">
         <v>46</v>
@@ -14318,7 +14318,7 @@
         <v>13.95</v>
       </c>
       <c r="W194" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X194" s="10" t="s">
         <v>46</v>
@@ -14386,7 +14386,7 @@
         <v>13.95</v>
       </c>
       <c r="W195" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X195" s="10" t="s">
         <v>46</v>
@@ -14454,7 +14454,7 @@
         <v>13.95</v>
       </c>
       <c r="W196" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X196" s="10" t="s">
         <v>46</v>
@@ -14522,7 +14522,7 @@
         <v>13.95</v>
       </c>
       <c r="W197" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X197" s="10" t="s">
         <v>46</v>
@@ -14590,7 +14590,7 @@
         <v>13.95</v>
       </c>
       <c r="W198" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X198" s="10" t="s">
         <v>46</v>
@@ -14658,7 +14658,7 @@
         <v>13.95</v>
       </c>
       <c r="W199" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X199" s="10" t="s">
         <v>46</v>
@@ -14726,7 +14726,7 @@
         <v>13.95</v>
       </c>
       <c r="W200" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X200" s="10" t="s">
         <v>46</v>
@@ -14794,7 +14794,7 @@
         <v>13.95</v>
       </c>
       <c r="W201" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X201" s="10" t="s">
         <v>46</v>
@@ -14862,10 +14862,10 @@
         <v>21</v>
       </c>
       <c r="W202" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X202" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="203" spans="1:24" x14ac:dyDescent="0.2">
@@ -14930,10 +14930,10 @@
         <v>21</v>
       </c>
       <c r="W203" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X203" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="204" spans="1:24" x14ac:dyDescent="0.2">
@@ -14998,10 +14998,10 @@
         <v>21</v>
       </c>
       <c r="W204" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X204" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="205" spans="1:24" x14ac:dyDescent="0.2">
@@ -15066,10 +15066,10 @@
         <v>21</v>
       </c>
       <c r="W205" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X205" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="206" spans="1:24" x14ac:dyDescent="0.2">
@@ -15134,10 +15134,10 @@
         <v>21</v>
       </c>
       <c r="W206" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X206" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="207" spans="1:24" x14ac:dyDescent="0.2">
@@ -15202,10 +15202,10 @@
         <v>21</v>
       </c>
       <c r="W207" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X207" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="208" spans="1:24" x14ac:dyDescent="0.2">
@@ -15270,10 +15270,10 @@
         <v>21</v>
       </c>
       <c r="W208" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X208" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="209" spans="1:24" x14ac:dyDescent="0.2">
@@ -15338,10 +15338,10 @@
         <v>21</v>
       </c>
       <c r="W209" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X209" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="210" spans="1:24" x14ac:dyDescent="0.2">
@@ -15406,10 +15406,10 @@
         <v>21</v>
       </c>
       <c r="W210" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X210" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="211" spans="1:24" x14ac:dyDescent="0.2">
@@ -15474,10 +15474,10 @@
         <v>21</v>
       </c>
       <c r="W211" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X211" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="212" spans="1:24" x14ac:dyDescent="0.2">
@@ -15542,10 +15542,10 @@
         <v>21</v>
       </c>
       <c r="W212" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X212" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="213" spans="1:24" x14ac:dyDescent="0.2">
@@ -15610,10 +15610,10 @@
         <v>21</v>
       </c>
       <c r="W213" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X213" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="214" spans="1:24" x14ac:dyDescent="0.2">
@@ -15678,10 +15678,10 @@
         <v>21</v>
       </c>
       <c r="W214" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X214" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="215" spans="1:24" x14ac:dyDescent="0.2">
@@ -15746,10 +15746,10 @@
         <v>21</v>
       </c>
       <c r="W215" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X215" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="216" spans="1:24" x14ac:dyDescent="0.2">
@@ -15814,10 +15814,10 @@
         <v>21</v>
       </c>
       <c r="W216" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X216" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="217" spans="1:24" x14ac:dyDescent="0.2">
@@ -15882,7 +15882,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W217" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X217" s="10" t="s">
         <v>92</v>
@@ -15950,7 +15950,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W218" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X218" s="10" t="s">
         <v>92</v>
@@ -16018,7 +16018,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W219" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X219" s="10" t="s">
         <v>92</v>
@@ -16086,7 +16086,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W220" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X220" s="10" t="s">
         <v>92</v>
@@ -16154,7 +16154,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W221" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X221" s="10" t="s">
         <v>92</v>
@@ -16222,7 +16222,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W222" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X222" s="10" t="s">
         <v>92</v>
@@ -16290,7 +16290,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W223" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X223" s="10" t="s">
         <v>92</v>
@@ -16358,7 +16358,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W224" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X224" s="10" t="s">
         <v>92</v>
@@ -16426,7 +16426,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W225" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X225" s="10" t="s">
         <v>92</v>
@@ -16494,7 +16494,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W226" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X226" s="10" t="s">
         <v>92</v>
@@ -16562,7 +16562,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W227" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X227" s="10" t="s">
         <v>92</v>
@@ -16630,7 +16630,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W228" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X228" s="10" t="s">
         <v>92</v>

</xml_diff>